<commit_message>
add back excel template version for import agent file
</commit_message>
<xml_diff>
--- a/front/src/assets/Fiche_agent_template.xlsx
+++ b/front/src/assets/Fiche_agent_template.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774B3F86-9D7C-1D4A-8912-7DB291CC5027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FF288F-367B-C547-A38E-235B7925990E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="22940" windowHeight="13320" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Formulaire à remplir" sheetId="6" r:id="rId1"/>
-    <sheet name="Calculatrice - Magistrats" sheetId="9" r:id="rId2"/>
-    <sheet name="Calculatrice - Fonctionnaires" sheetId="10" r:id="rId3"/>
-    <sheet name="Reconvertir un pourcentage" sheetId="11" r:id="rId4"/>
-    <sheet name="Fonction" sheetId="8" state="hidden" r:id="rId5"/>
+    <sheet name="Fonction" sheetId="8" state="hidden" r:id="rId2"/>
+    <sheet name="Calculatrice - Magistrats" sheetId="9" r:id="rId3"/>
+    <sheet name="Calculatrice - Fonctionnaires" sheetId="10" r:id="rId4"/>
+    <sheet name="Reconvertir un pourcentage" sheetId="11" r:id="rId5"/>
     <sheet name="Listes" sheetId="7" state="hidden" r:id="rId6"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Fonction!$A$1:$C$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Fonction!$A$1:$C$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1951,10 +1951,91 @@
     <xf numFmtId="0" fontId="12" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="12" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="4" fontId="12" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1974,11 +2055,26 @@
     <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="12" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1986,27 +2082,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2015,6 +2090,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2024,86 +2102,8 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4217,12 +4217,12 @@
     </row>
     <row r="6" spans="1:7" ht="56" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="50"/>
-      <c r="B6" s="81" t="s">
+      <c r="B6" s="108" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="81"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="82"/>
+      <c r="C6" s="108"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="109"/>
       <c r="F6" s="53"/>
     </row>
     <row r="7" spans="1:7" ht="110" customHeight="1" thickTop="1">
@@ -4247,8 +4247,8 @@
       <c r="B8" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="83"/>
-      <c r="D8" s="84"/>
+      <c r="C8" s="110"/>
+      <c r="D8" s="111"/>
       <c r="E8" s="74" t="s">
         <v>63</v>
       </c>
@@ -4258,7 +4258,7 @@
       <c r="A9" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="85" t="s">
+      <c r="B9" s="112" t="s">
         <v>65</v>
       </c>
       <c r="C9" s="59" t="s">
@@ -4272,7 +4272,7 @@
       <c r="A10" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="85"/>
+      <c r="B10" s="112"/>
       <c r="C10" s="59" t="s">
         <v>68</v>
       </c>
@@ -4284,7 +4284,7 @@
       <c r="A11" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="85"/>
+      <c r="B11" s="112"/>
       <c r="C11" s="59" t="s">
         <v>70</v>
       </c>
@@ -4296,7 +4296,7 @@
       <c r="A12" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="85"/>
+      <c r="B12" s="112"/>
       <c r="C12" s="59" t="s">
         <v>72</v>
       </c>
@@ -4323,7 +4323,7 @@
       <c r="A14" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B14" s="79" t="s">
+      <c r="B14" s="107" t="s">
         <v>76</v>
       </c>
       <c r="C14" s="59" t="s">
@@ -4337,7 +4337,7 @@
       <c r="A15" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="80"/>
+      <c r="B15" s="105"/>
       <c r="C15" s="59" t="s">
         <v>79</v>
       </c>
@@ -4349,7 +4349,7 @@
       <c r="A16" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B16" s="80"/>
+      <c r="B16" s="105"/>
       <c r="C16" s="59" t="s">
         <v>81</v>
       </c>
@@ -4361,7 +4361,7 @@
       <c r="A17" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="80"/>
+      <c r="B17" s="105"/>
       <c r="C17" s="59" t="s">
         <v>83</v>
       </c>
@@ -4373,7 +4373,7 @@
       <c r="A18" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B18" s="80"/>
+      <c r="B18" s="105"/>
       <c r="C18" s="59" t="s">
         <v>85</v>
       </c>
@@ -4385,7 +4385,7 @@
       <c r="A19" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="80"/>
+      <c r="B19" s="105"/>
       <c r="C19" s="59" t="s">
         <v>87</v>
       </c>
@@ -4397,7 +4397,7 @@
       <c r="A20" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="80"/>
+      <c r="B20" s="105"/>
       <c r="C20" s="59" t="s">
         <v>89</v>
       </c>
@@ -4409,7 +4409,7 @@
       <c r="A21" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="80"/>
+      <c r="B21" s="105"/>
       <c r="C21" s="59" t="s">
         <v>91</v>
       </c>
@@ -4421,7 +4421,7 @@
       <c r="A22" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B22" s="80"/>
+      <c r="B22" s="105"/>
       <c r="C22" s="59" t="s">
         <v>93</v>
       </c>
@@ -4448,7 +4448,7 @@
       <c r="A24" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="B24" s="79" t="s">
+      <c r="B24" s="107" t="s">
         <v>97</v>
       </c>
       <c r="C24" s="59" t="s">
@@ -4462,7 +4462,7 @@
       <c r="A25" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="B25" s="80"/>
+      <c r="B25" s="105"/>
       <c r="C25" s="59" t="s">
         <v>100</v>
       </c>
@@ -4474,7 +4474,7 @@
       <c r="A26" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="B26" s="80"/>
+      <c r="B26" s="105"/>
       <c r="C26" s="59" t="s">
         <v>102</v>
       </c>
@@ -4486,7 +4486,7 @@
       <c r="A27" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="B27" s="80"/>
+      <c r="B27" s="105"/>
       <c r="C27" s="59" t="s">
         <v>104</v>
       </c>
@@ -4498,7 +4498,7 @@
       <c r="A28" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="B28" s="80"/>
+      <c r="B28" s="105"/>
       <c r="C28" s="59" t="s">
         <v>106</v>
       </c>
@@ -4510,7 +4510,7 @@
       <c r="A29" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="B29" s="80"/>
+      <c r="B29" s="105"/>
       <c r="C29" s="59" t="s">
         <v>108</v>
       </c>
@@ -4522,7 +4522,7 @@
       <c r="A30" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="B30" s="80"/>
+      <c r="B30" s="105"/>
       <c r="C30" s="59" t="s">
         <v>70</v>
       </c>
@@ -4534,7 +4534,7 @@
       <c r="A31" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="B31" s="80"/>
+      <c r="B31" s="105"/>
       <c r="C31" s="59" t="s">
         <v>111</v>
       </c>
@@ -4561,7 +4561,7 @@
       <c r="A33" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="B33" s="79" t="s">
+      <c r="B33" s="107" t="s">
         <v>115</v>
       </c>
       <c r="C33" s="59" t="s">
@@ -4575,7 +4575,7 @@
       <c r="A34" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="B34" s="80"/>
+      <c r="B34" s="105"/>
       <c r="C34" s="59" t="s">
         <v>118</v>
       </c>
@@ -4587,7 +4587,7 @@
       <c r="A35" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="80"/>
+      <c r="B35" s="105"/>
       <c r="C35" s="59" t="s">
         <v>120</v>
       </c>
@@ -4599,7 +4599,7 @@
       <c r="A36" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="B36" s="80"/>
+      <c r="B36" s="105"/>
       <c r="C36" s="59" t="s">
         <v>122</v>
       </c>
@@ -4611,7 +4611,7 @@
       <c r="A37" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="B37" s="80"/>
+      <c r="B37" s="105"/>
       <c r="C37" s="59" t="s">
         <v>124</v>
       </c>
@@ -4623,7 +4623,7 @@
       <c r="A38" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="B38" s="80"/>
+      <c r="B38" s="105"/>
       <c r="C38" s="59" t="s">
         <v>126</v>
       </c>
@@ -4635,7 +4635,7 @@
       <c r="A39" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="B39" s="80"/>
+      <c r="B39" s="105"/>
       <c r="C39" s="59" t="s">
         <v>128</v>
       </c>
@@ -4647,7 +4647,7 @@
       <c r="A40" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="B40" s="80"/>
+      <c r="B40" s="105"/>
       <c r="C40" s="59" t="s">
         <v>130</v>
       </c>
@@ -4659,7 +4659,7 @@
       <c r="A41" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B41" s="80"/>
+      <c r="B41" s="105"/>
       <c r="C41" s="59" t="s">
         <v>132</v>
       </c>
@@ -4671,7 +4671,7 @@
       <c r="A42" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="B42" s="80"/>
+      <c r="B42" s="105"/>
       <c r="C42" s="59" t="s">
         <v>134</v>
       </c>
@@ -4683,7 +4683,7 @@
       <c r="A43" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="B43" s="80"/>
+      <c r="B43" s="105"/>
       <c r="C43" s="59" t="s">
         <v>136</v>
       </c>
@@ -4695,7 +4695,7 @@
       <c r="A44" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="B44" s="80"/>
+      <c r="B44" s="105"/>
       <c r="C44" s="59" t="s">
         <v>138</v>
       </c>
@@ -4707,7 +4707,7 @@
       <c r="A45" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="B45" s="80"/>
+      <c r="B45" s="105"/>
       <c r="C45" s="59" t="s">
         <v>140</v>
       </c>
@@ -4719,7 +4719,7 @@
       <c r="A46" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="B46" s="80"/>
+      <c r="B46" s="105"/>
       <c r="C46" s="59" t="s">
         <v>142</v>
       </c>
@@ -4731,7 +4731,7 @@
       <c r="A47" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="B47" s="80"/>
+      <c r="B47" s="105"/>
       <c r="C47" s="59" t="s">
         <v>144</v>
       </c>
@@ -4743,7 +4743,7 @@
       <c r="A48" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="B48" s="80"/>
+      <c r="B48" s="105"/>
       <c r="C48" s="59" t="s">
         <v>146</v>
       </c>
@@ -4755,7 +4755,7 @@
       <c r="A49" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="B49" s="80"/>
+      <c r="B49" s="105"/>
       <c r="C49" s="59" t="s">
         <v>148</v>
       </c>
@@ -4767,7 +4767,7 @@
       <c r="A50" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="B50" s="80"/>
+      <c r="B50" s="105"/>
       <c r="C50" s="59" t="s">
         <v>150</v>
       </c>
@@ -4779,7 +4779,7 @@
       <c r="A51" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="B51" s="80"/>
+      <c r="B51" s="105"/>
       <c r="C51" s="59" t="s">
         <v>152</v>
       </c>
@@ -4806,7 +4806,7 @@
       <c r="A53" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="B53" s="86" t="s">
+      <c r="B53" s="104" t="s">
         <v>156</v>
       </c>
       <c r="C53" s="59" t="s">
@@ -4820,7 +4820,7 @@
       <c r="A54" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="B54" s="80"/>
+      <c r="B54" s="105"/>
       <c r="C54" s="59" t="s">
         <v>159</v>
       </c>
@@ -4832,7 +4832,7 @@
       <c r="A55" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="B55" s="80"/>
+      <c r="B55" s="105"/>
       <c r="C55" s="59" t="s">
         <v>161</v>
       </c>
@@ -4859,7 +4859,7 @@
       <c r="A57" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="B57" s="79" t="s">
+      <c r="B57" s="107" t="s">
         <v>165</v>
       </c>
       <c r="C57" s="59" t="s">
@@ -4873,7 +4873,7 @@
       <c r="A58" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="B58" s="80"/>
+      <c r="B58" s="105"/>
       <c r="C58" s="59" t="s">
         <v>168</v>
       </c>
@@ -4900,7 +4900,7 @@
       <c r="A60" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="B60" s="79" t="s">
+      <c r="B60" s="107" t="s">
         <v>172</v>
       </c>
       <c r="C60" s="59" t="s">
@@ -4914,7 +4914,7 @@
       <c r="A61" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="B61" s="80"/>
+      <c r="B61" s="105"/>
       <c r="C61" s="59" t="s">
         <v>175</v>
       </c>
@@ -4926,7 +4926,7 @@
       <c r="A62" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="B62" s="80"/>
+      <c r="B62" s="105"/>
       <c r="C62" s="59" t="s">
         <v>177</v>
       </c>
@@ -4938,7 +4938,7 @@
       <c r="A63" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="B63" s="80"/>
+      <c r="B63" s="105"/>
       <c r="C63" s="59" t="s">
         <v>179</v>
       </c>
@@ -4950,7 +4950,7 @@
       <c r="A64" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="B64" s="80"/>
+      <c r="B64" s="105"/>
       <c r="C64" s="59" t="s">
         <v>181</v>
       </c>
@@ -4962,7 +4962,7 @@
       <c r="A65" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="B65" s="80"/>
+      <c r="B65" s="105"/>
       <c r="C65" s="59" t="s">
         <v>183</v>
       </c>
@@ -4974,7 +4974,7 @@
       <c r="A66" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="B66" s="80"/>
+      <c r="B66" s="105"/>
       <c r="C66" s="59" t="s">
         <v>185</v>
       </c>
@@ -4986,7 +4986,7 @@
       <c r="A67" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="B67" s="80"/>
+      <c r="B67" s="105"/>
       <c r="C67" s="59" t="s">
         <v>187</v>
       </c>
@@ -4998,7 +4998,7 @@
       <c r="A68" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="B68" s="80"/>
+      <c r="B68" s="105"/>
       <c r="C68" s="59" t="s">
         <v>189</v>
       </c>
@@ -5010,7 +5010,7 @@
       <c r="A69" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="B69" s="80"/>
+      <c r="B69" s="105"/>
       <c r="C69" s="59" t="s">
         <v>191</v>
       </c>
@@ -5022,7 +5022,7 @@
       <c r="A70" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="B70" s="80"/>
+      <c r="B70" s="105"/>
       <c r="C70" s="59" t="s">
         <v>193</v>
       </c>
@@ -5034,7 +5034,7 @@
       <c r="A71" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="B71" s="80"/>
+      <c r="B71" s="105"/>
       <c r="C71" s="59" t="s">
         <v>195</v>
       </c>
@@ -5046,7 +5046,7 @@
       <c r="A72" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="B72" s="80"/>
+      <c r="B72" s="105"/>
       <c r="C72" s="59" t="s">
         <v>197</v>
       </c>
@@ -5058,7 +5058,7 @@
       <c r="A73" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="B73" s="80"/>
+      <c r="B73" s="105"/>
       <c r="C73" s="59" t="s">
         <v>199</v>
       </c>
@@ -5070,7 +5070,7 @@
       <c r="A74" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="B74" s="80"/>
+      <c r="B74" s="105"/>
       <c r="C74" s="59" t="s">
         <v>201</v>
       </c>
@@ -5082,7 +5082,7 @@
       <c r="A75" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="B75" s="80"/>
+      <c r="B75" s="105"/>
       <c r="C75" s="59" t="s">
         <v>203</v>
       </c>
@@ -5109,7 +5109,7 @@
       <c r="A77" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="B77" s="86" t="s">
+      <c r="B77" s="104" t="s">
         <v>207</v>
       </c>
       <c r="C77" s="59" t="s">
@@ -5123,7 +5123,7 @@
       <c r="A78" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="B78" s="80"/>
+      <c r="B78" s="105"/>
       <c r="C78" s="59" t="s">
         <v>210</v>
       </c>
@@ -5135,7 +5135,7 @@
       <c r="A79" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="B79" s="80"/>
+      <c r="B79" s="105"/>
       <c r="C79" s="59" t="s">
         <v>212</v>
       </c>
@@ -5147,7 +5147,7 @@
       <c r="A80" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="B80" s="80"/>
+      <c r="B80" s="105"/>
       <c r="C80" s="59" t="s">
         <v>214</v>
       </c>
@@ -5159,7 +5159,7 @@
       <c r="A81" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="B81" s="80"/>
+      <c r="B81" s="105"/>
       <c r="C81" s="59" t="s">
         <v>216</v>
       </c>
@@ -5186,7 +5186,7 @@
       <c r="A83" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="B83" s="86" t="s">
+      <c r="B83" s="104" t="s">
         <v>220</v>
       </c>
       <c r="C83" s="59" t="s">
@@ -5200,7 +5200,7 @@
       <c r="A84" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="B84" s="80"/>
+      <c r="B84" s="105"/>
       <c r="C84" s="59" t="s">
         <v>223</v>
       </c>
@@ -5212,7 +5212,7 @@
       <c r="A85" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="B85" s="80"/>
+      <c r="B85" s="105"/>
       <c r="C85" s="59" t="s">
         <v>225</v>
       </c>
@@ -5224,7 +5224,7 @@
       <c r="A86" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="B86" s="80"/>
+      <c r="B86" s="105"/>
       <c r="C86" s="59" t="s">
         <v>227</v>
       </c>
@@ -5251,7 +5251,7 @@
       <c r="A88" s="12" t="s">
         <v>230</v>
       </c>
-      <c r="B88" s="86" t="s">
+      <c r="B88" s="104" t="s">
         <v>231</v>
       </c>
       <c r="C88" s="59" t="s">
@@ -5265,7 +5265,7 @@
       <c r="A89" s="12" t="s">
         <v>233</v>
       </c>
-      <c r="B89" s="80"/>
+      <c r="B89" s="105"/>
       <c r="C89" s="59" t="s">
         <v>234</v>
       </c>
@@ -5292,7 +5292,7 @@
       <c r="A91" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="B91" s="86" t="s">
+      <c r="B91" s="104" t="s">
         <v>238</v>
       </c>
       <c r="C91" s="59" t="s">
@@ -5306,7 +5306,7 @@
       <c r="A92" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="B92" s="80"/>
+      <c r="B92" s="105"/>
       <c r="C92" s="59" t="s">
         <v>241</v>
       </c>
@@ -5318,7 +5318,7 @@
       <c r="A93" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="B93" s="80"/>
+      <c r="B93" s="105"/>
       <c r="C93" s="59" t="s">
         <v>243</v>
       </c>
@@ -5330,7 +5330,7 @@
       <c r="A94" s="12" t="s">
         <v>244</v>
       </c>
-      <c r="B94" s="80"/>
+      <c r="B94" s="105"/>
       <c r="C94" s="59" t="s">
         <v>245</v>
       </c>
@@ -5342,7 +5342,7 @@
       <c r="A95" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="B95" s="80"/>
+      <c r="B95" s="105"/>
       <c r="C95" s="59" t="s">
         <v>247</v>
       </c>
@@ -5354,7 +5354,7 @@
       <c r="A96" s="12" t="s">
         <v>248</v>
       </c>
-      <c r="B96" s="80"/>
+      <c r="B96" s="105"/>
       <c r="C96" s="59" t="s">
         <v>249</v>
       </c>
@@ -5366,7 +5366,7 @@
       <c r="A97" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="B97" s="80"/>
+      <c r="B97" s="105"/>
       <c r="C97" s="59" t="s">
         <v>251</v>
       </c>
@@ -5407,10 +5407,10 @@
     <row r="101" spans="1:6">
       <c r="A101" s="12"/>
       <c r="B101" s="64"/>
-      <c r="C101" s="87" t="s">
+      <c r="C101" s="106" t="s">
         <v>255</v>
       </c>
-      <c r="D101" s="87"/>
+      <c r="D101" s="106"/>
       <c r="E101" s="60"/>
       <c r="F101" s="53"/>
     </row>
@@ -5453,6 +5453,12 @@
   <sheetProtection algorithmName="SHA-512" hashValue="InmqKlhhVhE+dGbIYDiSRnLE+IlAZxdLfnctzqDZDARVCn6iziD6wICeby41lmvE4W1J88KUyAnY0y7x+sw6lQ==" saltValue="K8srq741x0YFfj6gj3u+2g==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="14">
+    <mergeCell ref="B33:B51"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B14:B22"/>
+    <mergeCell ref="B24:B31"/>
     <mergeCell ref="B91:B97"/>
     <mergeCell ref="C101:D101"/>
     <mergeCell ref="B53:B55"/>
@@ -5461,12 +5467,6 @@
     <mergeCell ref="B77:B81"/>
     <mergeCell ref="B83:B86"/>
     <mergeCell ref="B88:B89"/>
-    <mergeCell ref="B33:B51"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B14:B22"/>
-    <mergeCell ref="B24:B31"/>
   </mergeCells>
   <conditionalFormatting sqref="B23">
     <cfRule type="expression" dxfId="13" priority="13">
@@ -5572,6 +5572,599 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDA0C244-7B66-A641-BA73-0F4A09F039A7}">
+  <dimension ref="A1:M27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScale="125" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="78" customWidth="1"/>
+    <col min="9" max="9" width="32" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="69" t="s">
+        <v>260</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>261</v>
+      </c>
+      <c r="C1" s="70" t="s">
+        <v>262</v>
+      </c>
+      <c r="E1" s="69" t="s">
+        <v>260</v>
+      </c>
+      <c r="F1" s="69" t="s">
+        <v>261</v>
+      </c>
+      <c r="G1" s="70" t="s">
+        <v>262</v>
+      </c>
+      <c r="H1" s="70"/>
+      <c r="I1" s="69" t="s">
+        <v>260</v>
+      </c>
+      <c r="J1" s="69" t="s">
+        <v>261</v>
+      </c>
+      <c r="K1" s="70" t="s">
+        <v>262</v>
+      </c>
+      <c r="M1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C2" s="71">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>265</v>
+      </c>
+      <c r="F2" t="s">
+        <v>265</v>
+      </c>
+      <c r="G2" s="72">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>266</v>
+      </c>
+      <c r="J2" t="s">
+        <v>267</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="M2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>268</v>
+      </c>
+      <c r="B3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C3" s="71">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>270</v>
+      </c>
+      <c r="F3" t="s">
+        <v>271</v>
+      </c>
+      <c r="G3" s="72">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>272</v>
+      </c>
+      <c r="J3" t="s">
+        <v>273</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="M3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>274</v>
+      </c>
+      <c r="B4" t="s">
+        <v>275</v>
+      </c>
+      <c r="C4" s="71">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>276</v>
+      </c>
+      <c r="F4" t="s">
+        <v>277</v>
+      </c>
+      <c r="G4" s="72">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>278</v>
+      </c>
+      <c r="J4" t="s">
+        <v>279</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>280</v>
+      </c>
+      <c r="B5" t="s">
+        <v>281</v>
+      </c>
+      <c r="C5" s="71">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>282</v>
+      </c>
+      <c r="F5" t="s">
+        <v>282</v>
+      </c>
+      <c r="G5" s="72">
+        <v>2</v>
+      </c>
+      <c r="I5" t="s">
+        <v>283</v>
+      </c>
+      <c r="J5" t="s">
+        <v>284</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>285</v>
+      </c>
+      <c r="B6" t="s">
+        <v>286</v>
+      </c>
+      <c r="C6" s="71">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>287</v>
+      </c>
+      <c r="F6" t="s">
+        <v>287</v>
+      </c>
+      <c r="G6" s="72">
+        <v>2</v>
+      </c>
+      <c r="I6" t="s">
+        <v>288</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>289</v>
+      </c>
+      <c r="B7" t="s">
+        <v>290</v>
+      </c>
+      <c r="C7" s="71">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>291</v>
+      </c>
+      <c r="F7" t="s">
+        <v>291</v>
+      </c>
+      <c r="G7" s="72">
+        <v>2</v>
+      </c>
+      <c r="I7" t="s">
+        <v>292</v>
+      </c>
+      <c r="K7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>293</v>
+      </c>
+      <c r="B8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C8" s="71">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>295</v>
+      </c>
+      <c r="F8" t="s">
+        <v>295</v>
+      </c>
+      <c r="G8" s="72">
+        <v>2</v>
+      </c>
+      <c r="I8" t="s">
+        <v>292</v>
+      </c>
+      <c r="K8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>296</v>
+      </c>
+      <c r="B9" t="s">
+        <v>297</v>
+      </c>
+      <c r="C9" s="71">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>298</v>
+      </c>
+      <c r="F9" t="s">
+        <v>299</v>
+      </c>
+      <c r="G9" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>300</v>
+      </c>
+      <c r="B10" t="s">
+        <v>301</v>
+      </c>
+      <c r="C10" s="71">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>302</v>
+      </c>
+      <c r="F10" t="s">
+        <v>302</v>
+      </c>
+      <c r="G10" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>303</v>
+      </c>
+      <c r="B11" t="s">
+        <v>304</v>
+      </c>
+      <c r="C11" s="71">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>305</v>
+      </c>
+      <c r="F11" t="s">
+        <v>305</v>
+      </c>
+      <c r="G11" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>306</v>
+      </c>
+      <c r="B12" t="s">
+        <v>307</v>
+      </c>
+      <c r="C12" s="71">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>308</v>
+      </c>
+      <c r="F12" t="s">
+        <v>308</v>
+      </c>
+      <c r="G12" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>309</v>
+      </c>
+      <c r="B13" t="s">
+        <v>310</v>
+      </c>
+      <c r="C13" s="71">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>311</v>
+      </c>
+      <c r="F13" t="s">
+        <v>312</v>
+      </c>
+      <c r="G13" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>313</v>
+      </c>
+      <c r="B14" t="s">
+        <v>314</v>
+      </c>
+      <c r="C14" s="71">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>315</v>
+      </c>
+      <c r="F14" t="s">
+        <v>316</v>
+      </c>
+      <c r="G14" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" t="s">
+        <v>317</v>
+      </c>
+      <c r="B15" t="s">
+        <v>318</v>
+      </c>
+      <c r="C15" s="71">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>319</v>
+      </c>
+      <c r="F15" t="s">
+        <v>320</v>
+      </c>
+      <c r="G15" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" t="s">
+        <v>321</v>
+      </c>
+      <c r="B16" t="s">
+        <v>322</v>
+      </c>
+      <c r="C16" s="71">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>323</v>
+      </c>
+      <c r="F16" t="s">
+        <v>324</v>
+      </c>
+      <c r="G16" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>325</v>
+      </c>
+      <c r="B17" t="s">
+        <v>326</v>
+      </c>
+      <c r="C17" s="71">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>327</v>
+      </c>
+      <c r="F17" t="s">
+        <v>328</v>
+      </c>
+      <c r="G17" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>329</v>
+      </c>
+      <c r="B18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="71">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>330</v>
+      </c>
+      <c r="F18" t="s">
+        <v>331</v>
+      </c>
+      <c r="G18" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>332</v>
+      </c>
+      <c r="B19" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19" s="71">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>333</v>
+      </c>
+      <c r="F19" t="s">
+        <v>334</v>
+      </c>
+      <c r="G19" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>335</v>
+      </c>
+      <c r="B20" t="s">
+        <v>207</v>
+      </c>
+      <c r="C20" s="71">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>288</v>
+      </c>
+      <c r="F20" t="s">
+        <v>336</v>
+      </c>
+      <c r="G20" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>337</v>
+      </c>
+      <c r="B21" t="s">
+        <v>220</v>
+      </c>
+      <c r="C21" s="71">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>292</v>
+      </c>
+      <c r="F21" t="s">
+        <v>338</v>
+      </c>
+      <c r="G21" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>339</v>
+      </c>
+      <c r="B22" t="s">
+        <v>340</v>
+      </c>
+      <c r="C22" s="71">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>341</v>
+      </c>
+      <c r="F22" t="s">
+        <v>342</v>
+      </c>
+      <c r="G22" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>343</v>
+      </c>
+      <c r="B23" t="s">
+        <v>344</v>
+      </c>
+      <c r="C23" s="71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>345</v>
+      </c>
+      <c r="B24" t="s">
+        <v>346</v>
+      </c>
+      <c r="C24" s="71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>347</v>
+      </c>
+      <c r="B25" t="s">
+        <v>348</v>
+      </c>
+      <c r="C25" s="71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>349</v>
+      </c>
+      <c r="B26" t="s">
+        <v>350</v>
+      </c>
+      <c r="C26" s="71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>351</v>
+      </c>
+      <c r="B27" t="s">
+        <v>352</v>
+      </c>
+      <c r="C27" s="71">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="afnDKsKrLmBaXS7c0wssz32egTAxgWv+IM9ZWJzya8iUE/HxESdpcrTiqLR7WxdNy50vR1vf/qx1SgLFL9+d1g==" saltValue="hd51xTYpDHe5+SlbhsdmJw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{849B8E3C-684A-A84E-BF7D-C966FE421893}">
   <dimension ref="B1:J19"/>
   <sheetViews>
@@ -5624,10 +6217,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="29"/>
-      <c r="F4" s="93" t="s">
+      <c r="F4" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="94"/>
+      <c r="G4" s="114"/>
       <c r="H4" s="1">
         <v>208</v>
       </c>
@@ -5636,10 +6229,10 @@
       </c>
     </row>
     <row r="5" spans="2:10" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1">
-      <c r="F5" s="95" t="s">
+      <c r="F5" s="115" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="96"/>
+      <c r="G5" s="116"/>
       <c r="H5" s="42">
         <v>8</v>
       </c>
@@ -5652,26 +6245,26 @@
       <c r="G6" s="40"/>
     </row>
     <row r="7" spans="2:10" ht="70" customHeight="1">
-      <c r="B7" s="91" t="s">
+      <c r="B7" s="117" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="19"/>
-      <c r="E7" s="90" t="s">
+      <c r="E7" s="119" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="90"/>
+      <c r="F7" s="119"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="88" t="s">
+      <c r="H7" s="120" t="s">
         <v>20</v>
       </c>
       <c r="J7"/>
     </row>
     <row r="8" spans="2:10" ht="26" customHeight="1">
-      <c r="B8" s="92"/>
-      <c r="H8" s="89"/>
+      <c r="B8" s="118"/>
+      <c r="H8" s="121"/>
       <c r="J8"/>
     </row>
     <row r="9" spans="2:10" ht="38.25" customHeight="1">
@@ -5708,7 +6301,7 @@
       <c r="J11"/>
     </row>
     <row r="12" spans="2:10" ht="69" customHeight="1">
-      <c r="B12" s="91" t="s">
+      <c r="B12" s="117" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="37" t="s">
@@ -5723,11 +6316,11 @@
       <c r="J12"/>
     </row>
     <row r="13" spans="2:10" ht="34.5" customHeight="1">
-      <c r="B13" s="92"/>
+      <c r="B13" s="118"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="9"/>
-      <c r="G13" s="89" t="s">
+      <c r="G13" s="121" t="s">
         <v>21</v>
       </c>
       <c r="J13"/>
@@ -5741,7 +6334,7 @@
       <c r="E14" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="89"/>
+      <c r="G14" s="121"/>
     </row>
     <row r="15" spans="2:10" s="3" customFormat="1" ht="6.75" customHeight="1">
       <c r="B15" s="17"/>
@@ -5787,13 +6380,13 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="nQ8joA74Rsh2Kx3Wfl1MFY2uo8GlElYBj87kqHVIo37r55P2tUu/gqoh5+2Pc6vWI/gF3F4U69Fb3n3B58JSQQ==" saltValue="TyXrh0FDS1+0gOHNSzrziQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="7">
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="G13:G14"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="H7:H8"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="G13:G14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5801,7 +6394,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CAF82AE-1CA4-9248-A03A-599FF8D211A8}">
   <dimension ref="B1:J19"/>
   <sheetViews>
@@ -5842,12 +6435,12 @@
         <v>1</v>
       </c>
       <c r="D3" s="28"/>
-      <c r="F3" s="97" t="s">
+      <c r="F3" s="122" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="99"/>
+      <c r="G3" s="123"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="124"/>
       <c r="J3"/>
     </row>
     <row r="4" spans="2:10" s="3" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
@@ -5856,10 +6449,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="29"/>
-      <c r="F4" s="93" t="s">
+      <c r="F4" s="113" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="94"/>
+      <c r="G4" s="114"/>
       <c r="H4" s="1">
         <v>1607</v>
       </c>
@@ -5868,10 +6461,10 @@
       </c>
     </row>
     <row r="5" spans="2:10" s="3" customFormat="1" ht="24.75" customHeight="1" thickBot="1">
-      <c r="F5" s="95" t="s">
+      <c r="F5" s="115" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="96"/>
+      <c r="G5" s="116"/>
       <c r="H5" s="39">
         <v>35</v>
       </c>
@@ -5886,26 +6479,26 @@
       </c>
     </row>
     <row r="7" spans="2:10" ht="70" customHeight="1">
-      <c r="B7" s="91" t="s">
+      <c r="B7" s="117" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="19"/>
-      <c r="E7" s="90" t="s">
+      <c r="E7" s="119" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="90"/>
+      <c r="F7" s="119"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="88" t="s">
+      <c r="H7" s="120" t="s">
         <v>20</v>
       </c>
       <c r="J7"/>
     </row>
     <row r="8" spans="2:10" ht="26" customHeight="1">
-      <c r="B8" s="92"/>
-      <c r="H8" s="89"/>
+      <c r="B8" s="118"/>
+      <c r="H8" s="121"/>
       <c r="J8"/>
     </row>
     <row r="9" spans="2:10" ht="38.25" customHeight="1">
@@ -5942,7 +6535,7 @@
       <c r="J11"/>
     </row>
     <row r="12" spans="2:10" ht="69" customHeight="1">
-      <c r="B12" s="91" t="s">
+      <c r="B12" s="117" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="37" t="s">
@@ -5957,11 +6550,11 @@
       <c r="J12"/>
     </row>
     <row r="13" spans="2:10" ht="34.5" customHeight="1">
-      <c r="B13" s="92"/>
+      <c r="B13" s="118"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="9"/>
-      <c r="G13" s="89" t="s">
+      <c r="G13" s="121" t="s">
         <v>21</v>
       </c>
       <c r="J13"/>
@@ -5975,7 +6568,7 @@
       <c r="E14" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="89"/>
+      <c r="G14" s="121"/>
     </row>
     <row r="15" spans="2:10" s="3" customFormat="1" ht="6.75" customHeight="1">
       <c r="B15" s="17"/>
@@ -6036,7 +6629,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63E04E73-8FDE-A94C-85C3-DA30BE340A9A}">
   <dimension ref="C1:I18"/>
   <sheetViews>
@@ -6051,7 +6644,7 @@
     <col min="3" max="3" width="43.5" style="46" customWidth="1"/>
     <col min="4" max="4" width="9" style="3" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" style="12" customWidth="1"/>
-    <col min="6" max="6" width="4" style="103" customWidth="1"/>
+    <col min="6" max="6" width="4" style="79" customWidth="1"/>
     <col min="7" max="7" width="6.6640625" style="3" customWidth="1"/>
     <col min="8" max="8" width="11.33203125" style="3"/>
     <col min="9" max="9" width="22.33203125" style="3" customWidth="1"/>
@@ -6064,32 +6657,32 @@
       <c r="F1" s="3"/>
     </row>
     <row r="2" spans="3:9" ht="54.75" customHeight="1">
-      <c r="C2" s="102" t="s">
+      <c r="C2" s="125" t="s">
         <v>355</v>
       </c>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="125"/>
+      <c r="F2" s="125"/>
+      <c r="G2" s="125"/>
+      <c r="H2" s="125"/>
+      <c r="I2" s="125"/>
     </row>
     <row r="3" spans="3:9" ht="27.75" customHeight="1">
       <c r="C3" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="100" t="s">
+      <c r="D3" s="126" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="101"/>
-      <c r="G3" s="104" t="s">
+      <c r="E3" s="127"/>
+      <c r="G3" s="128" t="s">
         <v>356</v>
       </c>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
+      <c r="H3" s="128"/>
+      <c r="I3" s="128"/>
     </row>
     <row r="4" spans="3:9" ht="23.25" customHeight="1">
-      <c r="C4" s="105" t="s">
+      <c r="C4" s="80" t="s">
         <v>357</v>
       </c>
       <c r="D4" s="43" t="str">
@@ -6098,14 +6691,14 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="53"/>
-      <c r="G4" s="103"/>
+      <c r="G4" s="79"/>
     </row>
     <row r="5" spans="3:9" ht="7.5" customHeight="1">
       <c r="C5" s="47"/>
       <c r="D5" s="43"/>
       <c r="E5" s="3"/>
       <c r="F5" s="12"/>
-      <c r="G5" s="103"/>
+      <c r="G5" s="79"/>
     </row>
     <row r="6" spans="3:9" ht="23.25" customHeight="1">
       <c r="C6" s="47" t="s">
@@ -6116,20 +6709,20 @@
         <v>42</v>
       </c>
       <c r="F6" s="12"/>
-      <c r="G6" s="103"/>
-      <c r="H6" s="106"/>
-      <c r="I6" s="106"/>
+      <c r="G6" s="79"/>
+      <c r="H6" s="81"/>
+      <c r="I6" s="81"/>
     </row>
     <row r="7" spans="3:9" ht="25.25" customHeight="1">
       <c r="C7" s="47"/>
-      <c r="D7" s="107" t="s">
+      <c r="D7" s="82" t="s">
         <v>358</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="12"/>
-      <c r="G7" s="108"/>
-      <c r="H7" s="106"/>
-      <c r="I7" s="106"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="81"/>
+      <c r="I7" s="81"/>
     </row>
     <row r="8" spans="3:9" ht="24" customHeight="1">
       <c r="C8" s="47" t="s">
@@ -6140,20 +6733,20 @@
         <v>44</v>
       </c>
       <c r="F8" s="12"/>
-      <c r="G8" s="103"/>
-      <c r="H8" s="106"/>
-      <c r="I8" s="106"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="81"/>
+      <c r="I8" s="81"/>
     </row>
     <row r="9" spans="3:9" ht="18" customHeight="1">
       <c r="C9" s="47"/>
-      <c r="D9" s="109" t="s">
+      <c r="D9" s="84" t="s">
         <v>359</v>
       </c>
       <c r="E9" s="48"/>
       <c r="F9" s="12"/>
-      <c r="G9" s="103"/>
-      <c r="H9" s="106"/>
-      <c r="I9" s="106"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="81"/>
+      <c r="I9" s="81"/>
     </row>
     <row r="10" spans="3:9" ht="36" customHeight="1">
       <c r="C10" s="47"/>
@@ -6162,33 +6755,33 @@
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="3:9" ht="24" customHeight="1">
-      <c r="C11" s="110" t="s">
+      <c r="C11" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="111">
+      <c r="D11" s="86">
         <f>IF(D3="MAGISTRAT",D6*D8*[1]Listes!D3,D6*D8*[1]Fonctionnaires!H4/7)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="112" t="s">
+      <c r="E11" s="87" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="113" t="s">
+      <c r="F11" s="88" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="114">
+      <c r="G11" s="89">
         <f>IF(D3="FONCTIONNAIRE",D11*7,D11*8)</f>
         <v>0</v>
       </c>
-      <c r="H11" s="112" t="s">
+      <c r="H11" s="87" t="s">
         <v>46</v>
       </c>
-      <c r="I11" s="115"/>
+      <c r="I11" s="90"/>
     </row>
     <row r="12" spans="3:9" ht="24" customHeight="1">
-      <c r="C12" s="116" t="s">
+      <c r="C12" s="91" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="117">
+      <c r="D12" s="92">
         <f>D11/12</f>
         <v>0</v>
       </c>
@@ -6198,56 +6791,56 @@
       <c r="F12" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="118">
+      <c r="G12" s="93">
         <f>IF(D4="FONCTIONNAIRE",D12*7,D12*8)</f>
         <v>0</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="I12" s="119"/>
+      <c r="I12" s="94"/>
     </row>
     <row r="13" spans="3:9" ht="24" customHeight="1">
-      <c r="C13" s="120" t="s">
+      <c r="C13" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="121">
+      <c r="D13" s="96">
         <f>(D8*D6)*5</f>
         <v>0</v>
       </c>
-      <c r="E13" s="122" t="s">
+      <c r="E13" s="97" t="s">
         <v>362</v>
       </c>
-      <c r="F13" s="123" t="s">
+      <c r="F13" s="98" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="124">
+      <c r="G13" s="99">
         <f>IF(D3="FONCTIONNAIRE",D13*7,D13*8)</f>
         <v>0</v>
       </c>
-      <c r="H13" s="122" t="s">
+      <c r="H13" s="97" t="s">
         <v>363</v>
       </c>
-      <c r="I13" s="125"/>
+      <c r="I13" s="100"/>
     </row>
     <row r="14" spans="3:9" ht="16.25" customHeight="1">
-      <c r="C14" s="126" t="s">
+      <c r="C14" s="101" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="15" spans="3:9" ht="16.25" customHeight="1">
-      <c r="C15" s="126" t="s">
+      <c r="C15" s="101" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="16" spans="3:9" ht="24" customHeight="1">
-      <c r="C16" s="127"/>
+      <c r="C16" s="102"/>
     </row>
     <row r="17" spans="3:3" ht="24" customHeight="1">
-      <c r="C17" s="128"/>
+      <c r="C17" s="103"/>
     </row>
     <row r="18" spans="3:3" ht="24" customHeight="1">
-      <c r="C18" s="127"/>
+      <c r="C18" s="102"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="Gy5QNriGlaVHeAjPum4cM0C4+yAHxmDli0jwulpHKqegGEbXID+fQiRrC1N4zJrSKGFxFCw3CH18lQT24sk6Nw==" saltValue="wVeS2Y8bMsGjmNDXNpg93A==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
@@ -6259,599 +6852,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDA0C244-7B66-A641-BA73-0F4A09F039A7}">
-  <dimension ref="A1:M27"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="125" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="78" customWidth="1"/>
-    <col min="9" max="9" width="32" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="69" t="s">
-        <v>260</v>
-      </c>
-      <c r="B1" s="69" t="s">
-        <v>261</v>
-      </c>
-      <c r="C1" s="70" t="s">
-        <v>262</v>
-      </c>
-      <c r="E1" s="69" t="s">
-        <v>260</v>
-      </c>
-      <c r="F1" s="69" t="s">
-        <v>261</v>
-      </c>
-      <c r="G1" s="70" t="s">
-        <v>262</v>
-      </c>
-      <c r="H1" s="70"/>
-      <c r="I1" s="69" t="s">
-        <v>260</v>
-      </c>
-      <c r="J1" s="69" t="s">
-        <v>261</v>
-      </c>
-      <c r="K1" s="70" t="s">
-        <v>262</v>
-      </c>
-      <c r="M1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" t="s">
-        <v>263</v>
-      </c>
-      <c r="B2" t="s">
-        <v>264</v>
-      </c>
-      <c r="C2" s="71">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>265</v>
-      </c>
-      <c r="F2" t="s">
-        <v>265</v>
-      </c>
-      <c r="G2" s="72">
-        <v>2</v>
-      </c>
-      <c r="I2" t="s">
-        <v>266</v>
-      </c>
-      <c r="J2" t="s">
-        <v>267</v>
-      </c>
-      <c r="K2">
-        <v>3</v>
-      </c>
-      <c r="M2" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" t="s">
-        <v>268</v>
-      </c>
-      <c r="B3" t="s">
-        <v>269</v>
-      </c>
-      <c r="C3" s="71">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>270</v>
-      </c>
-      <c r="F3" t="s">
-        <v>271</v>
-      </c>
-      <c r="G3" s="72">
-        <v>2</v>
-      </c>
-      <c r="I3" t="s">
-        <v>272</v>
-      </c>
-      <c r="J3" t="s">
-        <v>273</v>
-      </c>
-      <c r="K3">
-        <v>3</v>
-      </c>
-      <c r="M3" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" t="s">
-        <v>274</v>
-      </c>
-      <c r="B4" t="s">
-        <v>275</v>
-      </c>
-      <c r="C4" s="71">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F4" t="s">
-        <v>277</v>
-      </c>
-      <c r="G4" s="72">
-        <v>2</v>
-      </c>
-      <c r="I4" t="s">
-        <v>278</v>
-      </c>
-      <c r="J4" t="s">
-        <v>279</v>
-      </c>
-      <c r="K4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" t="s">
-        <v>280</v>
-      </c>
-      <c r="B5" t="s">
-        <v>281</v>
-      </c>
-      <c r="C5" s="71">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>282</v>
-      </c>
-      <c r="F5" t="s">
-        <v>282</v>
-      </c>
-      <c r="G5" s="72">
-        <v>2</v>
-      </c>
-      <c r="I5" t="s">
-        <v>283</v>
-      </c>
-      <c r="J5" t="s">
-        <v>284</v>
-      </c>
-      <c r="K5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" t="s">
-        <v>285</v>
-      </c>
-      <c r="B6" t="s">
-        <v>286</v>
-      </c>
-      <c r="C6" s="71">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>287</v>
-      </c>
-      <c r="F6" t="s">
-        <v>287</v>
-      </c>
-      <c r="G6" s="72">
-        <v>2</v>
-      </c>
-      <c r="I6" t="s">
-        <v>288</v>
-      </c>
-      <c r="K6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" t="s">
-        <v>289</v>
-      </c>
-      <c r="B7" t="s">
-        <v>290</v>
-      </c>
-      <c r="C7" s="71">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>291</v>
-      </c>
-      <c r="F7" t="s">
-        <v>291</v>
-      </c>
-      <c r="G7" s="72">
-        <v>2</v>
-      </c>
-      <c r="I7" t="s">
-        <v>292</v>
-      </c>
-      <c r="K7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" t="s">
-        <v>293</v>
-      </c>
-      <c r="B8" t="s">
-        <v>294</v>
-      </c>
-      <c r="C8" s="71">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>295</v>
-      </c>
-      <c r="F8" t="s">
-        <v>295</v>
-      </c>
-      <c r="G8" s="72">
-        <v>2</v>
-      </c>
-      <c r="I8" t="s">
-        <v>292</v>
-      </c>
-      <c r="K8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" t="s">
-        <v>296</v>
-      </c>
-      <c r="B9" t="s">
-        <v>297</v>
-      </c>
-      <c r="C9" s="71">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>298</v>
-      </c>
-      <c r="F9" t="s">
-        <v>299</v>
-      </c>
-      <c r="G9" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" t="s">
-        <v>300</v>
-      </c>
-      <c r="B10" t="s">
-        <v>301</v>
-      </c>
-      <c r="C10" s="71">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>302</v>
-      </c>
-      <c r="F10" t="s">
-        <v>302</v>
-      </c>
-      <c r="G10" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" t="s">
-        <v>303</v>
-      </c>
-      <c r="B11" t="s">
-        <v>304</v>
-      </c>
-      <c r="C11" s="71">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>305</v>
-      </c>
-      <c r="F11" t="s">
-        <v>305</v>
-      </c>
-      <c r="G11" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" t="s">
-        <v>306</v>
-      </c>
-      <c r="B12" t="s">
-        <v>307</v>
-      </c>
-      <c r="C12" s="71">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>308</v>
-      </c>
-      <c r="F12" t="s">
-        <v>308</v>
-      </c>
-      <c r="G12" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" t="s">
-        <v>309</v>
-      </c>
-      <c r="B13" t="s">
-        <v>310</v>
-      </c>
-      <c r="C13" s="71">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>311</v>
-      </c>
-      <c r="F13" t="s">
-        <v>312</v>
-      </c>
-      <c r="G13" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" t="s">
-        <v>313</v>
-      </c>
-      <c r="B14" t="s">
-        <v>314</v>
-      </c>
-      <c r="C14" s="71">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>315</v>
-      </c>
-      <c r="F14" t="s">
-        <v>316</v>
-      </c>
-      <c r="G14" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" t="s">
-        <v>317</v>
-      </c>
-      <c r="B15" t="s">
-        <v>318</v>
-      </c>
-      <c r="C15" s="71">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>319</v>
-      </c>
-      <c r="F15" t="s">
-        <v>320</v>
-      </c>
-      <c r="G15" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" t="s">
-        <v>321</v>
-      </c>
-      <c r="B16" t="s">
-        <v>322</v>
-      </c>
-      <c r="C16" s="71">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>323</v>
-      </c>
-      <c r="F16" t="s">
-        <v>324</v>
-      </c>
-      <c r="G16" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" t="s">
-        <v>325</v>
-      </c>
-      <c r="B17" t="s">
-        <v>326</v>
-      </c>
-      <c r="C17" s="71">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>327</v>
-      </c>
-      <c r="F17" t="s">
-        <v>328</v>
-      </c>
-      <c r="G17" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" t="s">
-        <v>329</v>
-      </c>
-      <c r="B18" t="s">
-        <v>97</v>
-      </c>
-      <c r="C18" s="71">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>330</v>
-      </c>
-      <c r="F18" t="s">
-        <v>331</v>
-      </c>
-      <c r="G18" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" t="s">
-        <v>332</v>
-      </c>
-      <c r="B19" t="s">
-        <v>165</v>
-      </c>
-      <c r="C19" s="71">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
-        <v>333</v>
-      </c>
-      <c r="F19" t="s">
-        <v>334</v>
-      </c>
-      <c r="G19" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" t="s">
-        <v>335</v>
-      </c>
-      <c r="B20" t="s">
-        <v>207</v>
-      </c>
-      <c r="C20" s="71">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>288</v>
-      </c>
-      <c r="F20" t="s">
-        <v>336</v>
-      </c>
-      <c r="G20" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" t="s">
-        <v>337</v>
-      </c>
-      <c r="B21" t="s">
-        <v>220</v>
-      </c>
-      <c r="C21" s="71">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>292</v>
-      </c>
-      <c r="F21" t="s">
-        <v>338</v>
-      </c>
-      <c r="G21" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" t="s">
-        <v>339</v>
-      </c>
-      <c r="B22" t="s">
-        <v>340</v>
-      </c>
-      <c r="C22" s="71">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
-        <v>341</v>
-      </c>
-      <c r="F22" t="s">
-        <v>342</v>
-      </c>
-      <c r="G22" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" t="s">
-        <v>343</v>
-      </c>
-      <c r="B23" t="s">
-        <v>344</v>
-      </c>
-      <c r="C23" s="71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" t="s">
-        <v>345</v>
-      </c>
-      <c r="B24" t="s">
-        <v>346</v>
-      </c>
-      <c r="C24" s="71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" t="s">
-        <v>347</v>
-      </c>
-      <c r="B25" t="s">
-        <v>348</v>
-      </c>
-      <c r="C25" s="71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" t="s">
-        <v>349</v>
-      </c>
-      <c r="B26" t="s">
-        <v>350</v>
-      </c>
-      <c r="C26" s="71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" t="s">
-        <v>351</v>
-      </c>
-      <c r="B27" t="s">
-        <v>352</v>
-      </c>
-      <c r="C27" s="71">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="afnDKsKrLmBaXS7c0wssz32egTAxgWv+IM9ZWJzya8iUE/HxESdpcrTiqLR7WxdNy50vR1vf/qx1SgLFL9+d1g==" saltValue="hd51xTYpDHe5+SlbhsdmJw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="3">
-    <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fix bug fiche agent - add back last excel file version
</commit_message>
<xml_diff>
--- a/front/src/assets/Fiche_agent_template.xlsx
+++ b/front/src/assets/Fiche_agent_template.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774B3F86-9D7C-1D4A-8912-7DB291CC5027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464B1286-445C-6D4F-9858-BA78EBD0330D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="22940" windowHeight="13320" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Formulaire à remplir" sheetId="6" r:id="rId1"/>
-    <sheet name="Calculatrice - Magistrats" sheetId="9" r:id="rId2"/>
-    <sheet name="Calculatrice - Fonctionnaires" sheetId="10" r:id="rId3"/>
-    <sheet name="Reconvertir un pourcentage" sheetId="11" r:id="rId4"/>
-    <sheet name="Fonction" sheetId="8" state="hidden" r:id="rId5"/>
+    <sheet name="Fonction" sheetId="8" state="hidden" r:id="rId2"/>
+    <sheet name="Calculatrice - Magistrats" sheetId="9" r:id="rId3"/>
+    <sheet name="Calculatrice - Fonctionnaires" sheetId="10" r:id="rId4"/>
+    <sheet name="Reconvertir un pourcentage" sheetId="11" r:id="rId5"/>
     <sheet name="Listes" sheetId="7" state="hidden" r:id="rId6"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Fonction!$A$1:$C$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Fonction!$A$1:$C$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1951,10 +1951,91 @@
     <xf numFmtId="0" fontId="12" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="12" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="4" fontId="12" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1974,11 +2055,26 @@
     <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="12" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1986,27 +2082,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2015,6 +2090,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2024,86 +2102,8 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4217,12 +4217,12 @@
     </row>
     <row r="6" spans="1:7" ht="56" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="50"/>
-      <c r="B6" s="81" t="s">
+      <c r="B6" s="108" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="81"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="82"/>
+      <c r="C6" s="108"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="109"/>
       <c r="F6" s="53"/>
     </row>
     <row r="7" spans="1:7" ht="110" customHeight="1" thickTop="1">
@@ -4247,8 +4247,8 @@
       <c r="B8" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="83"/>
-      <c r="D8" s="84"/>
+      <c r="C8" s="110"/>
+      <c r="D8" s="111"/>
       <c r="E8" s="74" t="s">
         <v>63</v>
       </c>
@@ -4258,7 +4258,7 @@
       <c r="A9" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="85" t="s">
+      <c r="B9" s="112" t="s">
         <v>65</v>
       </c>
       <c r="C9" s="59" t="s">
@@ -4272,7 +4272,7 @@
       <c r="A10" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="85"/>
+      <c r="B10" s="112"/>
       <c r="C10" s="59" t="s">
         <v>68</v>
       </c>
@@ -4284,7 +4284,7 @@
       <c r="A11" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="85"/>
+      <c r="B11" s="112"/>
       <c r="C11" s="59" t="s">
         <v>70</v>
       </c>
@@ -4296,7 +4296,7 @@
       <c r="A12" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="85"/>
+      <c r="B12" s="112"/>
       <c r="C12" s="59" t="s">
         <v>72</v>
       </c>
@@ -4323,7 +4323,7 @@
       <c r="A14" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B14" s="79" t="s">
+      <c r="B14" s="107" t="s">
         <v>76</v>
       </c>
       <c r="C14" s="59" t="s">
@@ -4337,7 +4337,7 @@
       <c r="A15" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="80"/>
+      <c r="B15" s="105"/>
       <c r="C15" s="59" t="s">
         <v>79</v>
       </c>
@@ -4349,7 +4349,7 @@
       <c r="A16" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B16" s="80"/>
+      <c r="B16" s="105"/>
       <c r="C16" s="59" t="s">
         <v>81</v>
       </c>
@@ -4361,7 +4361,7 @@
       <c r="A17" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="80"/>
+      <c r="B17" s="105"/>
       <c r="C17" s="59" t="s">
         <v>83</v>
       </c>
@@ -4373,7 +4373,7 @@
       <c r="A18" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B18" s="80"/>
+      <c r="B18" s="105"/>
       <c r="C18" s="59" t="s">
         <v>85</v>
       </c>
@@ -4385,7 +4385,7 @@
       <c r="A19" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="80"/>
+      <c r="B19" s="105"/>
       <c r="C19" s="59" t="s">
         <v>87</v>
       </c>
@@ -4397,7 +4397,7 @@
       <c r="A20" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="80"/>
+      <c r="B20" s="105"/>
       <c r="C20" s="59" t="s">
         <v>89</v>
       </c>
@@ -4409,7 +4409,7 @@
       <c r="A21" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="80"/>
+      <c r="B21" s="105"/>
       <c r="C21" s="59" t="s">
         <v>91</v>
       </c>
@@ -4421,7 +4421,7 @@
       <c r="A22" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B22" s="80"/>
+      <c r="B22" s="105"/>
       <c r="C22" s="59" t="s">
         <v>93</v>
       </c>
@@ -4448,7 +4448,7 @@
       <c r="A24" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="B24" s="79" t="s">
+      <c r="B24" s="107" t="s">
         <v>97</v>
       </c>
       <c r="C24" s="59" t="s">
@@ -4462,7 +4462,7 @@
       <c r="A25" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="B25" s="80"/>
+      <c r="B25" s="105"/>
       <c r="C25" s="59" t="s">
         <v>100</v>
       </c>
@@ -4474,7 +4474,7 @@
       <c r="A26" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="B26" s="80"/>
+      <c r="B26" s="105"/>
       <c r="C26" s="59" t="s">
         <v>102</v>
       </c>
@@ -4486,7 +4486,7 @@
       <c r="A27" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="B27" s="80"/>
+      <c r="B27" s="105"/>
       <c r="C27" s="59" t="s">
         <v>104</v>
       </c>
@@ -4498,7 +4498,7 @@
       <c r="A28" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="B28" s="80"/>
+      <c r="B28" s="105"/>
       <c r="C28" s="59" t="s">
         <v>106</v>
       </c>
@@ -4510,7 +4510,7 @@
       <c r="A29" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="B29" s="80"/>
+      <c r="B29" s="105"/>
       <c r="C29" s="59" t="s">
         <v>108</v>
       </c>
@@ -4522,7 +4522,7 @@
       <c r="A30" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="B30" s="80"/>
+      <c r="B30" s="105"/>
       <c r="C30" s="59" t="s">
         <v>70</v>
       </c>
@@ -4534,7 +4534,7 @@
       <c r="A31" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="B31" s="80"/>
+      <c r="B31" s="105"/>
       <c r="C31" s="59" t="s">
         <v>111</v>
       </c>
@@ -4561,7 +4561,7 @@
       <c r="A33" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="B33" s="79" t="s">
+      <c r="B33" s="107" t="s">
         <v>115</v>
       </c>
       <c r="C33" s="59" t="s">
@@ -4575,7 +4575,7 @@
       <c r="A34" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="B34" s="80"/>
+      <c r="B34" s="105"/>
       <c r="C34" s="59" t="s">
         <v>118</v>
       </c>
@@ -4587,7 +4587,7 @@
       <c r="A35" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="80"/>
+      <c r="B35" s="105"/>
       <c r="C35" s="59" t="s">
         <v>120</v>
       </c>
@@ -4599,7 +4599,7 @@
       <c r="A36" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="B36" s="80"/>
+      <c r="B36" s="105"/>
       <c r="C36" s="59" t="s">
         <v>122</v>
       </c>
@@ -4611,7 +4611,7 @@
       <c r="A37" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="B37" s="80"/>
+      <c r="B37" s="105"/>
       <c r="C37" s="59" t="s">
         <v>124</v>
       </c>
@@ -4623,7 +4623,7 @@
       <c r="A38" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="B38" s="80"/>
+      <c r="B38" s="105"/>
       <c r="C38" s="59" t="s">
         <v>126</v>
       </c>
@@ -4635,7 +4635,7 @@
       <c r="A39" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="B39" s="80"/>
+      <c r="B39" s="105"/>
       <c r="C39" s="59" t="s">
         <v>128</v>
       </c>
@@ -4647,7 +4647,7 @@
       <c r="A40" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="B40" s="80"/>
+      <c r="B40" s="105"/>
       <c r="C40" s="59" t="s">
         <v>130</v>
       </c>
@@ -4659,7 +4659,7 @@
       <c r="A41" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B41" s="80"/>
+      <c r="B41" s="105"/>
       <c r="C41" s="59" t="s">
         <v>132</v>
       </c>
@@ -4671,7 +4671,7 @@
       <c r="A42" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="B42" s="80"/>
+      <c r="B42" s="105"/>
       <c r="C42" s="59" t="s">
         <v>134</v>
       </c>
@@ -4683,7 +4683,7 @@
       <c r="A43" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="B43" s="80"/>
+      <c r="B43" s="105"/>
       <c r="C43" s="59" t="s">
         <v>136</v>
       </c>
@@ -4695,7 +4695,7 @@
       <c r="A44" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="B44" s="80"/>
+      <c r="B44" s="105"/>
       <c r="C44" s="59" t="s">
         <v>138</v>
       </c>
@@ -4707,7 +4707,7 @@
       <c r="A45" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="B45" s="80"/>
+      <c r="B45" s="105"/>
       <c r="C45" s="59" t="s">
         <v>140</v>
       </c>
@@ -4719,7 +4719,7 @@
       <c r="A46" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="B46" s="80"/>
+      <c r="B46" s="105"/>
       <c r="C46" s="59" t="s">
         <v>142</v>
       </c>
@@ -4731,7 +4731,7 @@
       <c r="A47" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="B47" s="80"/>
+      <c r="B47" s="105"/>
       <c r="C47" s="59" t="s">
         <v>144</v>
       </c>
@@ -4743,7 +4743,7 @@
       <c r="A48" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="B48" s="80"/>
+      <c r="B48" s="105"/>
       <c r="C48" s="59" t="s">
         <v>146</v>
       </c>
@@ -4755,7 +4755,7 @@
       <c r="A49" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="B49" s="80"/>
+      <c r="B49" s="105"/>
       <c r="C49" s="59" t="s">
         <v>148</v>
       </c>
@@ -4767,7 +4767,7 @@
       <c r="A50" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="B50" s="80"/>
+      <c r="B50" s="105"/>
       <c r="C50" s="59" t="s">
         <v>150</v>
       </c>
@@ -4779,7 +4779,7 @@
       <c r="A51" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="B51" s="80"/>
+      <c r="B51" s="105"/>
       <c r="C51" s="59" t="s">
         <v>152</v>
       </c>
@@ -4806,7 +4806,7 @@
       <c r="A53" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="B53" s="86" t="s">
+      <c r="B53" s="104" t="s">
         <v>156</v>
       </c>
       <c r="C53" s="59" t="s">
@@ -4820,7 +4820,7 @@
       <c r="A54" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="B54" s="80"/>
+      <c r="B54" s="105"/>
       <c r="C54" s="59" t="s">
         <v>159</v>
       </c>
@@ -4832,7 +4832,7 @@
       <c r="A55" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="B55" s="80"/>
+      <c r="B55" s="105"/>
       <c r="C55" s="59" t="s">
         <v>161</v>
       </c>
@@ -4859,7 +4859,7 @@
       <c r="A57" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="B57" s="79" t="s">
+      <c r="B57" s="107" t="s">
         <v>165</v>
       </c>
       <c r="C57" s="59" t="s">
@@ -4873,7 +4873,7 @@
       <c r="A58" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="B58" s="80"/>
+      <c r="B58" s="105"/>
       <c r="C58" s="59" t="s">
         <v>168</v>
       </c>
@@ -4900,7 +4900,7 @@
       <c r="A60" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="B60" s="79" t="s">
+      <c r="B60" s="107" t="s">
         <v>172</v>
       </c>
       <c r="C60" s="59" t="s">
@@ -4914,7 +4914,7 @@
       <c r="A61" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="B61" s="80"/>
+      <c r="B61" s="105"/>
       <c r="C61" s="59" t="s">
         <v>175</v>
       </c>
@@ -4926,7 +4926,7 @@
       <c r="A62" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="B62" s="80"/>
+      <c r="B62" s="105"/>
       <c r="C62" s="59" t="s">
         <v>177</v>
       </c>
@@ -4938,7 +4938,7 @@
       <c r="A63" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="B63" s="80"/>
+      <c r="B63" s="105"/>
       <c r="C63" s="59" t="s">
         <v>179</v>
       </c>
@@ -4950,7 +4950,7 @@
       <c r="A64" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="B64" s="80"/>
+      <c r="B64" s="105"/>
       <c r="C64" s="59" t="s">
         <v>181</v>
       </c>
@@ -4962,7 +4962,7 @@
       <c r="A65" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="B65" s="80"/>
+      <c r="B65" s="105"/>
       <c r="C65" s="59" t="s">
         <v>183</v>
       </c>
@@ -4974,7 +4974,7 @@
       <c r="A66" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="B66" s="80"/>
+      <c r="B66" s="105"/>
       <c r="C66" s="59" t="s">
         <v>185</v>
       </c>
@@ -4986,7 +4986,7 @@
       <c r="A67" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="B67" s="80"/>
+      <c r="B67" s="105"/>
       <c r="C67" s="59" t="s">
         <v>187</v>
       </c>
@@ -4998,7 +4998,7 @@
       <c r="A68" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="B68" s="80"/>
+      <c r="B68" s="105"/>
       <c r="C68" s="59" t="s">
         <v>189</v>
       </c>
@@ -5010,7 +5010,7 @@
       <c r="A69" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="B69" s="80"/>
+      <c r="B69" s="105"/>
       <c r="C69" s="59" t="s">
         <v>191</v>
       </c>
@@ -5022,7 +5022,7 @@
       <c r="A70" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="B70" s="80"/>
+      <c r="B70" s="105"/>
       <c r="C70" s="59" t="s">
         <v>193</v>
       </c>
@@ -5034,7 +5034,7 @@
       <c r="A71" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="B71" s="80"/>
+      <c r="B71" s="105"/>
       <c r="C71" s="59" t="s">
         <v>195</v>
       </c>
@@ -5046,7 +5046,7 @@
       <c r="A72" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="B72" s="80"/>
+      <c r="B72" s="105"/>
       <c r="C72" s="59" t="s">
         <v>197</v>
       </c>
@@ -5058,7 +5058,7 @@
       <c r="A73" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="B73" s="80"/>
+      <c r="B73" s="105"/>
       <c r="C73" s="59" t="s">
         <v>199</v>
       </c>
@@ -5070,7 +5070,7 @@
       <c r="A74" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="B74" s="80"/>
+      <c r="B74" s="105"/>
       <c r="C74" s="59" t="s">
         <v>201</v>
       </c>
@@ -5082,7 +5082,7 @@
       <c r="A75" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="B75" s="80"/>
+      <c r="B75" s="105"/>
       <c r="C75" s="59" t="s">
         <v>203</v>
       </c>
@@ -5109,7 +5109,7 @@
       <c r="A77" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="B77" s="86" t="s">
+      <c r="B77" s="104" t="s">
         <v>207</v>
       </c>
       <c r="C77" s="59" t="s">
@@ -5123,7 +5123,7 @@
       <c r="A78" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="B78" s="80"/>
+      <c r="B78" s="105"/>
       <c r="C78" s="59" t="s">
         <v>210</v>
       </c>
@@ -5135,7 +5135,7 @@
       <c r="A79" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="B79" s="80"/>
+      <c r="B79" s="105"/>
       <c r="C79" s="59" t="s">
         <v>212</v>
       </c>
@@ -5147,7 +5147,7 @@
       <c r="A80" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="B80" s="80"/>
+      <c r="B80" s="105"/>
       <c r="C80" s="59" t="s">
         <v>214</v>
       </c>
@@ -5159,7 +5159,7 @@
       <c r="A81" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="B81" s="80"/>
+      <c r="B81" s="105"/>
       <c r="C81" s="59" t="s">
         <v>216</v>
       </c>
@@ -5186,7 +5186,7 @@
       <c r="A83" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="B83" s="86" t="s">
+      <c r="B83" s="104" t="s">
         <v>220</v>
       </c>
       <c r="C83" s="59" t="s">
@@ -5200,7 +5200,7 @@
       <c r="A84" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="B84" s="80"/>
+      <c r="B84" s="105"/>
       <c r="C84" s="59" t="s">
         <v>223</v>
       </c>
@@ -5212,7 +5212,7 @@
       <c r="A85" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="B85" s="80"/>
+      <c r="B85" s="105"/>
       <c r="C85" s="59" t="s">
         <v>225</v>
       </c>
@@ -5224,7 +5224,7 @@
       <c r="A86" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="B86" s="80"/>
+      <c r="B86" s="105"/>
       <c r="C86" s="59" t="s">
         <v>227</v>
       </c>
@@ -5251,7 +5251,7 @@
       <c r="A88" s="12" t="s">
         <v>230</v>
       </c>
-      <c r="B88" s="86" t="s">
+      <c r="B88" s="104" t="s">
         <v>231</v>
       </c>
       <c r="C88" s="59" t="s">
@@ -5265,7 +5265,7 @@
       <c r="A89" s="12" t="s">
         <v>233</v>
       </c>
-      <c r="B89" s="80"/>
+      <c r="B89" s="105"/>
       <c r="C89" s="59" t="s">
         <v>234</v>
       </c>
@@ -5292,7 +5292,7 @@
       <c r="A91" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="B91" s="86" t="s">
+      <c r="B91" s="104" t="s">
         <v>238</v>
       </c>
       <c r="C91" s="59" t="s">
@@ -5306,7 +5306,7 @@
       <c r="A92" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="B92" s="80"/>
+      <c r="B92" s="105"/>
       <c r="C92" s="59" t="s">
         <v>241</v>
       </c>
@@ -5318,7 +5318,7 @@
       <c r="A93" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="B93" s="80"/>
+      <c r="B93" s="105"/>
       <c r="C93" s="59" t="s">
         <v>243</v>
       </c>
@@ -5330,7 +5330,7 @@
       <c r="A94" s="12" t="s">
         <v>244</v>
       </c>
-      <c r="B94" s="80"/>
+      <c r="B94" s="105"/>
       <c r="C94" s="59" t="s">
         <v>245</v>
       </c>
@@ -5342,7 +5342,7 @@
       <c r="A95" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="B95" s="80"/>
+      <c r="B95" s="105"/>
       <c r="C95" s="59" t="s">
         <v>247</v>
       </c>
@@ -5354,7 +5354,7 @@
       <c r="A96" s="12" t="s">
         <v>248</v>
       </c>
-      <c r="B96" s="80"/>
+      <c r="B96" s="105"/>
       <c r="C96" s="59" t="s">
         <v>249</v>
       </c>
@@ -5366,7 +5366,7 @@
       <c r="A97" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="B97" s="80"/>
+      <c r="B97" s="105"/>
       <c r="C97" s="59" t="s">
         <v>251</v>
       </c>
@@ -5407,10 +5407,10 @@
     <row r="101" spans="1:6">
       <c r="A101" s="12"/>
       <c r="B101" s="64"/>
-      <c r="C101" s="87" t="s">
+      <c r="C101" s="106" t="s">
         <v>255</v>
       </c>
-      <c r="D101" s="87"/>
+      <c r="D101" s="106"/>
       <c r="E101" s="60"/>
       <c r="F101" s="53"/>
     </row>
@@ -5453,6 +5453,12 @@
   <sheetProtection algorithmName="SHA-512" hashValue="InmqKlhhVhE+dGbIYDiSRnLE+IlAZxdLfnctzqDZDARVCn6iziD6wICeby41lmvE4W1J88KUyAnY0y7x+sw6lQ==" saltValue="K8srq741x0YFfj6gj3u+2g==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="14">
+    <mergeCell ref="B33:B51"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B14:B22"/>
+    <mergeCell ref="B24:B31"/>
     <mergeCell ref="B91:B97"/>
     <mergeCell ref="C101:D101"/>
     <mergeCell ref="B53:B55"/>
@@ -5461,12 +5467,6 @@
     <mergeCell ref="B77:B81"/>
     <mergeCell ref="B83:B86"/>
     <mergeCell ref="B88:B89"/>
-    <mergeCell ref="B33:B51"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B14:B22"/>
-    <mergeCell ref="B24:B31"/>
   </mergeCells>
   <conditionalFormatting sqref="B23">
     <cfRule type="expression" dxfId="13" priority="13">
@@ -5572,6 +5572,599 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDA0C244-7B66-A641-BA73-0F4A09F039A7}">
+  <dimension ref="A1:M27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScale="125" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="78" customWidth="1"/>
+    <col min="9" max="9" width="32" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="69" t="s">
+        <v>260</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>261</v>
+      </c>
+      <c r="C1" s="70" t="s">
+        <v>262</v>
+      </c>
+      <c r="E1" s="69" t="s">
+        <v>260</v>
+      </c>
+      <c r="F1" s="69" t="s">
+        <v>261</v>
+      </c>
+      <c r="G1" s="70" t="s">
+        <v>262</v>
+      </c>
+      <c r="H1" s="70"/>
+      <c r="I1" s="69" t="s">
+        <v>260</v>
+      </c>
+      <c r="J1" s="69" t="s">
+        <v>261</v>
+      </c>
+      <c r="K1" s="70" t="s">
+        <v>262</v>
+      </c>
+      <c r="M1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C2" s="71">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>265</v>
+      </c>
+      <c r="F2" t="s">
+        <v>265</v>
+      </c>
+      <c r="G2" s="72">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>266</v>
+      </c>
+      <c r="J2" t="s">
+        <v>267</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="M2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>268</v>
+      </c>
+      <c r="B3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C3" s="71">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>270</v>
+      </c>
+      <c r="F3" t="s">
+        <v>271</v>
+      </c>
+      <c r="G3" s="72">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>272</v>
+      </c>
+      <c r="J3" t="s">
+        <v>273</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="M3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>274</v>
+      </c>
+      <c r="B4" t="s">
+        <v>275</v>
+      </c>
+      <c r="C4" s="71">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>276</v>
+      </c>
+      <c r="F4" t="s">
+        <v>277</v>
+      </c>
+      <c r="G4" s="72">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>278</v>
+      </c>
+      <c r="J4" t="s">
+        <v>279</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>280</v>
+      </c>
+      <c r="B5" t="s">
+        <v>281</v>
+      </c>
+      <c r="C5" s="71">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>282</v>
+      </c>
+      <c r="F5" t="s">
+        <v>282</v>
+      </c>
+      <c r="G5" s="72">
+        <v>2</v>
+      </c>
+      <c r="I5" t="s">
+        <v>283</v>
+      </c>
+      <c r="J5" t="s">
+        <v>284</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>285</v>
+      </c>
+      <c r="B6" t="s">
+        <v>286</v>
+      </c>
+      <c r="C6" s="71">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>287</v>
+      </c>
+      <c r="F6" t="s">
+        <v>287</v>
+      </c>
+      <c r="G6" s="72">
+        <v>2</v>
+      </c>
+      <c r="I6" t="s">
+        <v>288</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>289</v>
+      </c>
+      <c r="B7" t="s">
+        <v>290</v>
+      </c>
+      <c r="C7" s="71">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>291</v>
+      </c>
+      <c r="F7" t="s">
+        <v>291</v>
+      </c>
+      <c r="G7" s="72">
+        <v>2</v>
+      </c>
+      <c r="I7" t="s">
+        <v>292</v>
+      </c>
+      <c r="K7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>293</v>
+      </c>
+      <c r="B8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C8" s="71">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>295</v>
+      </c>
+      <c r="F8" t="s">
+        <v>295</v>
+      </c>
+      <c r="G8" s="72">
+        <v>2</v>
+      </c>
+      <c r="I8" t="s">
+        <v>292</v>
+      </c>
+      <c r="K8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>296</v>
+      </c>
+      <c r="B9" t="s">
+        <v>297</v>
+      </c>
+      <c r="C9" s="71">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>298</v>
+      </c>
+      <c r="F9" t="s">
+        <v>299</v>
+      </c>
+      <c r="G9" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>300</v>
+      </c>
+      <c r="B10" t="s">
+        <v>301</v>
+      </c>
+      <c r="C10" s="71">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>302</v>
+      </c>
+      <c r="F10" t="s">
+        <v>302</v>
+      </c>
+      <c r="G10" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>303</v>
+      </c>
+      <c r="B11" t="s">
+        <v>304</v>
+      </c>
+      <c r="C11" s="71">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>305</v>
+      </c>
+      <c r="F11" t="s">
+        <v>305</v>
+      </c>
+      <c r="G11" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>306</v>
+      </c>
+      <c r="B12" t="s">
+        <v>307</v>
+      </c>
+      <c r="C12" s="71">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>308</v>
+      </c>
+      <c r="F12" t="s">
+        <v>308</v>
+      </c>
+      <c r="G12" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>309</v>
+      </c>
+      <c r="B13" t="s">
+        <v>310</v>
+      </c>
+      <c r="C13" s="71">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>311</v>
+      </c>
+      <c r="F13" t="s">
+        <v>312</v>
+      </c>
+      <c r="G13" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>313</v>
+      </c>
+      <c r="B14" t="s">
+        <v>314</v>
+      </c>
+      <c r="C14" s="71">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>315</v>
+      </c>
+      <c r="F14" t="s">
+        <v>316</v>
+      </c>
+      <c r="G14" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" t="s">
+        <v>317</v>
+      </c>
+      <c r="B15" t="s">
+        <v>318</v>
+      </c>
+      <c r="C15" s="71">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>319</v>
+      </c>
+      <c r="F15" t="s">
+        <v>320</v>
+      </c>
+      <c r="G15" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" t="s">
+        <v>321</v>
+      </c>
+      <c r="B16" t="s">
+        <v>322</v>
+      </c>
+      <c r="C16" s="71">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>323</v>
+      </c>
+      <c r="F16" t="s">
+        <v>324</v>
+      </c>
+      <c r="G16" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>325</v>
+      </c>
+      <c r="B17" t="s">
+        <v>326</v>
+      </c>
+      <c r="C17" s="71">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>327</v>
+      </c>
+      <c r="F17" t="s">
+        <v>328</v>
+      </c>
+      <c r="G17" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>329</v>
+      </c>
+      <c r="B18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="71">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>330</v>
+      </c>
+      <c r="F18" t="s">
+        <v>331</v>
+      </c>
+      <c r="G18" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>332</v>
+      </c>
+      <c r="B19" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19" s="71">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>333</v>
+      </c>
+      <c r="F19" t="s">
+        <v>334</v>
+      </c>
+      <c r="G19" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>335</v>
+      </c>
+      <c r="B20" t="s">
+        <v>207</v>
+      </c>
+      <c r="C20" s="71">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>288</v>
+      </c>
+      <c r="F20" t="s">
+        <v>336</v>
+      </c>
+      <c r="G20" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>337</v>
+      </c>
+      <c r="B21" t="s">
+        <v>220</v>
+      </c>
+      <c r="C21" s="71">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>292</v>
+      </c>
+      <c r="F21" t="s">
+        <v>338</v>
+      </c>
+      <c r="G21" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>339</v>
+      </c>
+      <c r="B22" t="s">
+        <v>340</v>
+      </c>
+      <c r="C22" s="71">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>341</v>
+      </c>
+      <c r="F22" t="s">
+        <v>342</v>
+      </c>
+      <c r="G22" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>343</v>
+      </c>
+      <c r="B23" t="s">
+        <v>344</v>
+      </c>
+      <c r="C23" s="71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>345</v>
+      </c>
+      <c r="B24" t="s">
+        <v>346</v>
+      </c>
+      <c r="C24" s="71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>347</v>
+      </c>
+      <c r="B25" t="s">
+        <v>348</v>
+      </c>
+      <c r="C25" s="71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>349</v>
+      </c>
+      <c r="B26" t="s">
+        <v>350</v>
+      </c>
+      <c r="C26" s="71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>351</v>
+      </c>
+      <c r="B27" t="s">
+        <v>352</v>
+      </c>
+      <c r="C27" s="71">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="afnDKsKrLmBaXS7c0wssz32egTAxgWv+IM9ZWJzya8iUE/HxESdpcrTiqLR7WxdNy50vR1vf/qx1SgLFL9+d1g==" saltValue="hd51xTYpDHe5+SlbhsdmJw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{849B8E3C-684A-A84E-BF7D-C966FE421893}">
   <dimension ref="B1:J19"/>
   <sheetViews>
@@ -5624,10 +6217,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="29"/>
-      <c r="F4" s="93" t="s">
+      <c r="F4" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="94"/>
+      <c r="G4" s="114"/>
       <c r="H4" s="1">
         <v>208</v>
       </c>
@@ -5636,10 +6229,10 @@
       </c>
     </row>
     <row r="5" spans="2:10" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1">
-      <c r="F5" s="95" t="s">
+      <c r="F5" s="115" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="96"/>
+      <c r="G5" s="116"/>
       <c r="H5" s="42">
         <v>8</v>
       </c>
@@ -5652,26 +6245,26 @@
       <c r="G6" s="40"/>
     </row>
     <row r="7" spans="2:10" ht="70" customHeight="1">
-      <c r="B7" s="91" t="s">
+      <c r="B7" s="117" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="19"/>
-      <c r="E7" s="90" t="s">
+      <c r="E7" s="119" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="90"/>
+      <c r="F7" s="119"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="88" t="s">
+      <c r="H7" s="120" t="s">
         <v>20</v>
       </c>
       <c r="J7"/>
     </row>
     <row r="8" spans="2:10" ht="26" customHeight="1">
-      <c r="B8" s="92"/>
-      <c r="H8" s="89"/>
+      <c r="B8" s="118"/>
+      <c r="H8" s="121"/>
       <c r="J8"/>
     </row>
     <row r="9" spans="2:10" ht="38.25" customHeight="1">
@@ -5708,7 +6301,7 @@
       <c r="J11"/>
     </row>
     <row r="12" spans="2:10" ht="69" customHeight="1">
-      <c r="B12" s="91" t="s">
+      <c r="B12" s="117" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="37" t="s">
@@ -5723,11 +6316,11 @@
       <c r="J12"/>
     </row>
     <row r="13" spans="2:10" ht="34.5" customHeight="1">
-      <c r="B13" s="92"/>
+      <c r="B13" s="118"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="9"/>
-      <c r="G13" s="89" t="s">
+      <c r="G13" s="121" t="s">
         <v>21</v>
       </c>
       <c r="J13"/>
@@ -5741,7 +6334,7 @@
       <c r="E14" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="89"/>
+      <c r="G14" s="121"/>
     </row>
     <row r="15" spans="2:10" s="3" customFormat="1" ht="6.75" customHeight="1">
       <c r="B15" s="17"/>
@@ -5787,13 +6380,13 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="nQ8joA74Rsh2Kx3Wfl1MFY2uo8GlElYBj87kqHVIo37r55P2tUu/gqoh5+2Pc6vWI/gF3F4U69Fb3n3B58JSQQ==" saltValue="TyXrh0FDS1+0gOHNSzrziQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="7">
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="G13:G14"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="H7:H8"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="G13:G14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5801,7 +6394,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CAF82AE-1CA4-9248-A03A-599FF8D211A8}">
   <dimension ref="B1:J19"/>
   <sheetViews>
@@ -5842,12 +6435,12 @@
         <v>1</v>
       </c>
       <c r="D3" s="28"/>
-      <c r="F3" s="97" t="s">
+      <c r="F3" s="122" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="99"/>
+      <c r="G3" s="123"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="124"/>
       <c r="J3"/>
     </row>
     <row r="4" spans="2:10" s="3" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
@@ -5856,10 +6449,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="29"/>
-      <c r="F4" s="93" t="s">
+      <c r="F4" s="113" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="94"/>
+      <c r="G4" s="114"/>
       <c r="H4" s="1">
         <v>1607</v>
       </c>
@@ -5868,10 +6461,10 @@
       </c>
     </row>
     <row r="5" spans="2:10" s="3" customFormat="1" ht="24.75" customHeight="1" thickBot="1">
-      <c r="F5" s="95" t="s">
+      <c r="F5" s="115" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="96"/>
+      <c r="G5" s="116"/>
       <c r="H5" s="39">
         <v>35</v>
       </c>
@@ -5886,26 +6479,26 @@
       </c>
     </row>
     <row r="7" spans="2:10" ht="70" customHeight="1">
-      <c r="B7" s="91" t="s">
+      <c r="B7" s="117" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="19"/>
-      <c r="E7" s="90" t="s">
+      <c r="E7" s="119" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="90"/>
+      <c r="F7" s="119"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="88" t="s">
+      <c r="H7" s="120" t="s">
         <v>20</v>
       </c>
       <c r="J7"/>
     </row>
     <row r="8" spans="2:10" ht="26" customHeight="1">
-      <c r="B8" s="92"/>
-      <c r="H8" s="89"/>
+      <c r="B8" s="118"/>
+      <c r="H8" s="121"/>
       <c r="J8"/>
     </row>
     <row r="9" spans="2:10" ht="38.25" customHeight="1">
@@ -5942,7 +6535,7 @@
       <c r="J11"/>
     </row>
     <row r="12" spans="2:10" ht="69" customHeight="1">
-      <c r="B12" s="91" t="s">
+      <c r="B12" s="117" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="37" t="s">
@@ -5957,11 +6550,11 @@
       <c r="J12"/>
     </row>
     <row r="13" spans="2:10" ht="34.5" customHeight="1">
-      <c r="B13" s="92"/>
+      <c r="B13" s="118"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="9"/>
-      <c r="G13" s="89" t="s">
+      <c r="G13" s="121" t="s">
         <v>21</v>
       </c>
       <c r="J13"/>
@@ -5975,7 +6568,7 @@
       <c r="E14" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="89"/>
+      <c r="G14" s="121"/>
     </row>
     <row r="15" spans="2:10" s="3" customFormat="1" ht="6.75" customHeight="1">
       <c r="B15" s="17"/>
@@ -6036,7 +6629,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63E04E73-8FDE-A94C-85C3-DA30BE340A9A}">
   <dimension ref="C1:I18"/>
   <sheetViews>
@@ -6051,7 +6644,7 @@
     <col min="3" max="3" width="43.5" style="46" customWidth="1"/>
     <col min="4" max="4" width="9" style="3" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" style="12" customWidth="1"/>
-    <col min="6" max="6" width="4" style="103" customWidth="1"/>
+    <col min="6" max="6" width="4" style="79" customWidth="1"/>
     <col min="7" max="7" width="6.6640625" style="3" customWidth="1"/>
     <col min="8" max="8" width="11.33203125" style="3"/>
     <col min="9" max="9" width="22.33203125" style="3" customWidth="1"/>
@@ -6064,32 +6657,32 @@
       <c r="F1" s="3"/>
     </row>
     <row r="2" spans="3:9" ht="54.75" customHeight="1">
-      <c r="C2" s="102" t="s">
+      <c r="C2" s="125" t="s">
         <v>355</v>
       </c>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="125"/>
+      <c r="F2" s="125"/>
+      <c r="G2" s="125"/>
+      <c r="H2" s="125"/>
+      <c r="I2" s="125"/>
     </row>
     <row r="3" spans="3:9" ht="27.75" customHeight="1">
       <c r="C3" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="100" t="s">
+      <c r="D3" s="126" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="101"/>
-      <c r="G3" s="104" t="s">
+      <c r="E3" s="127"/>
+      <c r="G3" s="128" t="s">
         <v>356</v>
       </c>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
+      <c r="H3" s="128"/>
+      <c r="I3" s="128"/>
     </row>
     <row r="4" spans="3:9" ht="23.25" customHeight="1">
-      <c r="C4" s="105" t="s">
+      <c r="C4" s="80" t="s">
         <v>357</v>
       </c>
       <c r="D4" s="43" t="str">
@@ -6098,14 +6691,14 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="53"/>
-      <c r="G4" s="103"/>
+      <c r="G4" s="79"/>
     </row>
     <row r="5" spans="3:9" ht="7.5" customHeight="1">
       <c r="C5" s="47"/>
       <c r="D5" s="43"/>
       <c r="E5" s="3"/>
       <c r="F5" s="12"/>
-      <c r="G5" s="103"/>
+      <c r="G5" s="79"/>
     </row>
     <row r="6" spans="3:9" ht="23.25" customHeight="1">
       <c r="C6" s="47" t="s">
@@ -6116,20 +6709,20 @@
         <v>42</v>
       </c>
       <c r="F6" s="12"/>
-      <c r="G6" s="103"/>
-      <c r="H6" s="106"/>
-      <c r="I6" s="106"/>
+      <c r="G6" s="79"/>
+      <c r="H6" s="81"/>
+      <c r="I6" s="81"/>
     </row>
     <row r="7" spans="3:9" ht="25.25" customHeight="1">
       <c r="C7" s="47"/>
-      <c r="D7" s="107" t="s">
+      <c r="D7" s="82" t="s">
         <v>358</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="12"/>
-      <c r="G7" s="108"/>
-      <c r="H7" s="106"/>
-      <c r="I7" s="106"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="81"/>
+      <c r="I7" s="81"/>
     </row>
     <row r="8" spans="3:9" ht="24" customHeight="1">
       <c r="C8" s="47" t="s">
@@ -6140,20 +6733,20 @@
         <v>44</v>
       </c>
       <c r="F8" s="12"/>
-      <c r="G8" s="103"/>
-      <c r="H8" s="106"/>
-      <c r="I8" s="106"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="81"/>
+      <c r="I8" s="81"/>
     </row>
     <row r="9" spans="3:9" ht="18" customHeight="1">
       <c r="C9" s="47"/>
-      <c r="D9" s="109" t="s">
+      <c r="D9" s="84" t="s">
         <v>359</v>
       </c>
       <c r="E9" s="48"/>
       <c r="F9" s="12"/>
-      <c r="G9" s="103"/>
-      <c r="H9" s="106"/>
-      <c r="I9" s="106"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="81"/>
+      <c r="I9" s="81"/>
     </row>
     <row r="10" spans="3:9" ht="36" customHeight="1">
       <c r="C10" s="47"/>
@@ -6162,33 +6755,33 @@
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="3:9" ht="24" customHeight="1">
-      <c r="C11" s="110" t="s">
+      <c r="C11" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="111">
+      <c r="D11" s="86">
         <f>IF(D3="MAGISTRAT",D6*D8*[1]Listes!D3,D6*D8*[1]Fonctionnaires!H4/7)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="112" t="s">
+      <c r="E11" s="87" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="113" t="s">
+      <c r="F11" s="88" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="114">
+      <c r="G11" s="89">
         <f>IF(D3="FONCTIONNAIRE",D11*7,D11*8)</f>
         <v>0</v>
       </c>
-      <c r="H11" s="112" t="s">
+      <c r="H11" s="87" t="s">
         <v>46</v>
       </c>
-      <c r="I11" s="115"/>
+      <c r="I11" s="90"/>
     </row>
     <row r="12" spans="3:9" ht="24" customHeight="1">
-      <c r="C12" s="116" t="s">
+      <c r="C12" s="91" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="117">
+      <c r="D12" s="92">
         <f>D11/12</f>
         <v>0</v>
       </c>
@@ -6198,56 +6791,56 @@
       <c r="F12" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="118">
+      <c r="G12" s="93">
         <f>IF(D4="FONCTIONNAIRE",D12*7,D12*8)</f>
         <v>0</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="I12" s="119"/>
+      <c r="I12" s="94"/>
     </row>
     <row r="13" spans="3:9" ht="24" customHeight="1">
-      <c r="C13" s="120" t="s">
+      <c r="C13" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="121">
+      <c r="D13" s="96">
         <f>(D8*D6)*5</f>
         <v>0</v>
       </c>
-      <c r="E13" s="122" t="s">
+      <c r="E13" s="97" t="s">
         <v>362</v>
       </c>
-      <c r="F13" s="123" t="s">
+      <c r="F13" s="98" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="124">
+      <c r="G13" s="99">
         <f>IF(D3="FONCTIONNAIRE",D13*7,D13*8)</f>
         <v>0</v>
       </c>
-      <c r="H13" s="122" t="s">
+      <c r="H13" s="97" t="s">
         <v>363</v>
       </c>
-      <c r="I13" s="125"/>
+      <c r="I13" s="100"/>
     </row>
     <row r="14" spans="3:9" ht="16.25" customHeight="1">
-      <c r="C14" s="126" t="s">
+      <c r="C14" s="101" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="15" spans="3:9" ht="16.25" customHeight="1">
-      <c r="C15" s="126" t="s">
+      <c r="C15" s="101" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="16" spans="3:9" ht="24" customHeight="1">
-      <c r="C16" s="127"/>
+      <c r="C16" s="102"/>
     </row>
     <row r="17" spans="3:3" ht="24" customHeight="1">
-      <c r="C17" s="128"/>
+      <c r="C17" s="103"/>
     </row>
     <row r="18" spans="3:3" ht="24" customHeight="1">
-      <c r="C18" s="127"/>
+      <c r="C18" s="102"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="Gy5QNriGlaVHeAjPum4cM0C4+yAHxmDli0jwulpHKqegGEbXID+fQiRrC1N4zJrSKGFxFCw3CH18lQT24sk6Nw==" saltValue="wVeS2Y8bMsGjmNDXNpg93A==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
@@ -6259,599 +6852,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDA0C244-7B66-A641-BA73-0F4A09F039A7}">
-  <dimension ref="A1:M27"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="125" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="78" customWidth="1"/>
-    <col min="9" max="9" width="32" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="69" t="s">
-        <v>260</v>
-      </c>
-      <c r="B1" s="69" t="s">
-        <v>261</v>
-      </c>
-      <c r="C1" s="70" t="s">
-        <v>262</v>
-      </c>
-      <c r="E1" s="69" t="s">
-        <v>260</v>
-      </c>
-      <c r="F1" s="69" t="s">
-        <v>261</v>
-      </c>
-      <c r="G1" s="70" t="s">
-        <v>262</v>
-      </c>
-      <c r="H1" s="70"/>
-      <c r="I1" s="69" t="s">
-        <v>260</v>
-      </c>
-      <c r="J1" s="69" t="s">
-        <v>261</v>
-      </c>
-      <c r="K1" s="70" t="s">
-        <v>262</v>
-      </c>
-      <c r="M1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" t="s">
-        <v>263</v>
-      </c>
-      <c r="B2" t="s">
-        <v>264</v>
-      </c>
-      <c r="C2" s="71">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>265</v>
-      </c>
-      <c r="F2" t="s">
-        <v>265</v>
-      </c>
-      <c r="G2" s="72">
-        <v>2</v>
-      </c>
-      <c r="I2" t="s">
-        <v>266</v>
-      </c>
-      <c r="J2" t="s">
-        <v>267</v>
-      </c>
-      <c r="K2">
-        <v>3</v>
-      </c>
-      <c r="M2" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" t="s">
-        <v>268</v>
-      </c>
-      <c r="B3" t="s">
-        <v>269</v>
-      </c>
-      <c r="C3" s="71">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>270</v>
-      </c>
-      <c r="F3" t="s">
-        <v>271</v>
-      </c>
-      <c r="G3" s="72">
-        <v>2</v>
-      </c>
-      <c r="I3" t="s">
-        <v>272</v>
-      </c>
-      <c r="J3" t="s">
-        <v>273</v>
-      </c>
-      <c r="K3">
-        <v>3</v>
-      </c>
-      <c r="M3" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" t="s">
-        <v>274</v>
-      </c>
-      <c r="B4" t="s">
-        <v>275</v>
-      </c>
-      <c r="C4" s="71">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F4" t="s">
-        <v>277</v>
-      </c>
-      <c r="G4" s="72">
-        <v>2</v>
-      </c>
-      <c r="I4" t="s">
-        <v>278</v>
-      </c>
-      <c r="J4" t="s">
-        <v>279</v>
-      </c>
-      <c r="K4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" t="s">
-        <v>280</v>
-      </c>
-      <c r="B5" t="s">
-        <v>281</v>
-      </c>
-      <c r="C5" s="71">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>282</v>
-      </c>
-      <c r="F5" t="s">
-        <v>282</v>
-      </c>
-      <c r="G5" s="72">
-        <v>2</v>
-      </c>
-      <c r="I5" t="s">
-        <v>283</v>
-      </c>
-      <c r="J5" t="s">
-        <v>284</v>
-      </c>
-      <c r="K5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" t="s">
-        <v>285</v>
-      </c>
-      <c r="B6" t="s">
-        <v>286</v>
-      </c>
-      <c r="C6" s="71">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>287</v>
-      </c>
-      <c r="F6" t="s">
-        <v>287</v>
-      </c>
-      <c r="G6" s="72">
-        <v>2</v>
-      </c>
-      <c r="I6" t="s">
-        <v>288</v>
-      </c>
-      <c r="K6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" t="s">
-        <v>289</v>
-      </c>
-      <c r="B7" t="s">
-        <v>290</v>
-      </c>
-      <c r="C7" s="71">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>291</v>
-      </c>
-      <c r="F7" t="s">
-        <v>291</v>
-      </c>
-      <c r="G7" s="72">
-        <v>2</v>
-      </c>
-      <c r="I7" t="s">
-        <v>292</v>
-      </c>
-      <c r="K7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" t="s">
-        <v>293</v>
-      </c>
-      <c r="B8" t="s">
-        <v>294</v>
-      </c>
-      <c r="C8" s="71">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>295</v>
-      </c>
-      <c r="F8" t="s">
-        <v>295</v>
-      </c>
-      <c r="G8" s="72">
-        <v>2</v>
-      </c>
-      <c r="I8" t="s">
-        <v>292</v>
-      </c>
-      <c r="K8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" t="s">
-        <v>296</v>
-      </c>
-      <c r="B9" t="s">
-        <v>297</v>
-      </c>
-      <c r="C9" s="71">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>298</v>
-      </c>
-      <c r="F9" t="s">
-        <v>299</v>
-      </c>
-      <c r="G9" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" t="s">
-        <v>300</v>
-      </c>
-      <c r="B10" t="s">
-        <v>301</v>
-      </c>
-      <c r="C10" s="71">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>302</v>
-      </c>
-      <c r="F10" t="s">
-        <v>302</v>
-      </c>
-      <c r="G10" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" t="s">
-        <v>303</v>
-      </c>
-      <c r="B11" t="s">
-        <v>304</v>
-      </c>
-      <c r="C11" s="71">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>305</v>
-      </c>
-      <c r="F11" t="s">
-        <v>305</v>
-      </c>
-      <c r="G11" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" t="s">
-        <v>306</v>
-      </c>
-      <c r="B12" t="s">
-        <v>307</v>
-      </c>
-      <c r="C12" s="71">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>308</v>
-      </c>
-      <c r="F12" t="s">
-        <v>308</v>
-      </c>
-      <c r="G12" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" t="s">
-        <v>309</v>
-      </c>
-      <c r="B13" t="s">
-        <v>310</v>
-      </c>
-      <c r="C13" s="71">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>311</v>
-      </c>
-      <c r="F13" t="s">
-        <v>312</v>
-      </c>
-      <c r="G13" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" t="s">
-        <v>313</v>
-      </c>
-      <c r="B14" t="s">
-        <v>314</v>
-      </c>
-      <c r="C14" s="71">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>315</v>
-      </c>
-      <c r="F14" t="s">
-        <v>316</v>
-      </c>
-      <c r="G14" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" t="s">
-        <v>317</v>
-      </c>
-      <c r="B15" t="s">
-        <v>318</v>
-      </c>
-      <c r="C15" s="71">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>319</v>
-      </c>
-      <c r="F15" t="s">
-        <v>320</v>
-      </c>
-      <c r="G15" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" t="s">
-        <v>321</v>
-      </c>
-      <c r="B16" t="s">
-        <v>322</v>
-      </c>
-      <c r="C16" s="71">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>323</v>
-      </c>
-      <c r="F16" t="s">
-        <v>324</v>
-      </c>
-      <c r="G16" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" t="s">
-        <v>325</v>
-      </c>
-      <c r="B17" t="s">
-        <v>326</v>
-      </c>
-      <c r="C17" s="71">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>327</v>
-      </c>
-      <c r="F17" t="s">
-        <v>328</v>
-      </c>
-      <c r="G17" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" t="s">
-        <v>329</v>
-      </c>
-      <c r="B18" t="s">
-        <v>97</v>
-      </c>
-      <c r="C18" s="71">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>330</v>
-      </c>
-      <c r="F18" t="s">
-        <v>331</v>
-      </c>
-      <c r="G18" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" t="s">
-        <v>332</v>
-      </c>
-      <c r="B19" t="s">
-        <v>165</v>
-      </c>
-      <c r="C19" s="71">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
-        <v>333</v>
-      </c>
-      <c r="F19" t="s">
-        <v>334</v>
-      </c>
-      <c r="G19" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" t="s">
-        <v>335</v>
-      </c>
-      <c r="B20" t="s">
-        <v>207</v>
-      </c>
-      <c r="C20" s="71">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>288</v>
-      </c>
-      <c r="F20" t="s">
-        <v>336</v>
-      </c>
-      <c r="G20" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" t="s">
-        <v>337</v>
-      </c>
-      <c r="B21" t="s">
-        <v>220</v>
-      </c>
-      <c r="C21" s="71">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>292</v>
-      </c>
-      <c r="F21" t="s">
-        <v>338</v>
-      </c>
-      <c r="G21" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" t="s">
-        <v>339</v>
-      </c>
-      <c r="B22" t="s">
-        <v>340</v>
-      </c>
-      <c r="C22" s="71">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
-        <v>341</v>
-      </c>
-      <c r="F22" t="s">
-        <v>342</v>
-      </c>
-      <c r="G22" s="72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" t="s">
-        <v>343</v>
-      </c>
-      <c r="B23" t="s">
-        <v>344</v>
-      </c>
-      <c r="C23" s="71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" t="s">
-        <v>345</v>
-      </c>
-      <c r="B24" t="s">
-        <v>346</v>
-      </c>
-      <c r="C24" s="71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" t="s">
-        <v>347</v>
-      </c>
-      <c r="B25" t="s">
-        <v>348</v>
-      </c>
-      <c r="C25" s="71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" t="s">
-        <v>349</v>
-      </c>
-      <c r="B26" t="s">
-        <v>350</v>
-      </c>
-      <c r="C26" s="71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" t="s">
-        <v>351</v>
-      </c>
-      <c r="B27" t="s">
-        <v>352</v>
-      </c>
-      <c r="C27" s="71">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="afnDKsKrLmBaXS7c0wssz32egTAxgWv+IM9ZWJzya8iUE/HxESdpcrTiqLR7WxdNy50vR1vf/qx1SgLFL9+d1g==" saltValue="hd51xTYpDHe5+SlbhsdmJw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="3">
-    <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
correction calculatrice fiche agent
</commit_message>
<xml_diff>
--- a/front/src/assets/Fiche_agent_template.xlsx
+++ b/front/src/assets/Fiche_agent_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FF288F-367B-C547-A38E-235B7925990E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693CACA0-2F1C-2A41-8590-67A7584D1189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="22940" windowHeight="13320" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17840" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Formulaire à remplir" sheetId="6" r:id="rId1"/>
@@ -22,6 +22,7 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Fonction!$A$1:$C$27</definedName>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="367">
   <si>
     <t>Temps de travail d'un magistrat</t>
   </si>
@@ -1226,6 +1227,9 @@
   </si>
   <si>
     <t>** étant considérée comme une semaine : une semaine pleine de 5 jours travaillés</t>
+  </si>
+  <si>
+    <t>FONCTIONNAIRE</t>
   </si>
 </sst>
 </file>
@@ -1928,7 +1932,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2026,16 +2029,10 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="12" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="12" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="12" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2055,6 +2052,21 @@
     <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="12" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -2067,19 +2079,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2105,6 +2108,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Milliers" xfId="2" builtinId="3"/>
@@ -3822,6 +3826,56 @@
 </externalLink>
 </file>
 
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Magistrats"/>
+      <sheetName val="Fonctionnaires"/>
+      <sheetName val="Reconvertir un pourcentage"/>
+      <sheetName val="Listes"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="4">
+          <cell r="H4">
+            <v>208</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="H5">
+            <v>8</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="4">
+          <cell r="H4">
+            <v>1607</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="H5">
+            <v>35</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3">
+        <row r="10">
+          <cell r="B10">
+            <v>7</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B99F57A7-32F2-EB4E-89DD-FC7B22582351}" name="GREFFE" displayName="GREFFE" ref="E1:E22" totalsRowShown="0" headerRowDxfId="16">
   <autoFilter ref="E1:E22" xr:uid="{5A6E512E-A730-F44B-89B8-85BBEC58376E}"/>
@@ -4172,7 +4226,7 @@
     </row>
     <row r="2" spans="1:7" ht="33" customHeight="1">
       <c r="A2" s="50"/>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="72" t="s">
         <v>53</v>
       </c>
       <c r="C2" s="51"/>
@@ -4183,7 +4237,7 @@
     </row>
     <row r="3" spans="1:7" ht="33" customHeight="1">
       <c r="A3" s="50"/>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="72" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="51"/>
@@ -4194,7 +4248,7 @@
     </row>
     <row r="4" spans="1:7" ht="33" customHeight="1">
       <c r="A4" s="50"/>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="72" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="51"/>
@@ -4205,11 +4259,11 @@
     </row>
     <row r="5" spans="1:7" ht="31" customHeight="1" thickBot="1">
       <c r="A5" s="50"/>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="72" t="s">
         <v>56</v>
       </c>
       <c r="C5" s="51"/>
-      <c r="D5" s="73" t="s">
+      <c r="D5" s="72" t="s">
         <v>57</v>
       </c>
       <c r="E5" s="55"/>
@@ -4217,26 +4271,26 @@
     </row>
     <row r="6" spans="1:7" ht="56" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="50"/>
-      <c r="B6" s="108" t="s">
+      <c r="B6" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="108"/>
-      <c r="D6" s="108"/>
-      <c r="E6" s="109"/>
+      <c r="C6" s="105"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="106"/>
       <c r="F6" s="53"/>
     </row>
     <row r="7" spans="1:7" ht="110" customHeight="1" thickTop="1">
       <c r="A7" s="12"/>
-      <c r="B7" s="75" t="s">
+      <c r="B7" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="75" t="s">
+      <c r="C7" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="76" t="s">
+      <c r="D7" s="75" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="77">
+      <c r="E7" s="76">
         <f>SUM(E102,E90,E87,E82,E76,E59,E56,E52,E32,E23,E13)/100</f>
         <v>0</v>
       </c>
@@ -4244,12 +4298,12 @@
     </row>
     <row r="8" spans="1:7" ht="42" customHeight="1" thickBot="1">
       <c r="A8" s="12"/>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="110"/>
-      <c r="D8" s="111"/>
-      <c r="E8" s="74" t="s">
+      <c r="C8" s="107"/>
+      <c r="D8" s="108"/>
+      <c r="E8" s="73" t="s">
         <v>63</v>
       </c>
       <c r="F8" s="53"/>
@@ -4258,7 +4312,7 @@
       <c r="A9" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="112" t="s">
+      <c r="B9" s="109" t="s">
         <v>65</v>
       </c>
       <c r="C9" s="59" t="s">
@@ -4272,7 +4326,7 @@
       <c r="A10" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="112"/>
+      <c r="B10" s="109"/>
       <c r="C10" s="59" t="s">
         <v>68</v>
       </c>
@@ -4284,7 +4338,7 @@
       <c r="A11" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="112"/>
+      <c r="B11" s="109"/>
       <c r="C11" s="59" t="s">
         <v>70</v>
       </c>
@@ -4296,7 +4350,7 @@
       <c r="A12" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="112"/>
+      <c r="B12" s="109"/>
       <c r="C12" s="59" t="s">
         <v>72</v>
       </c>
@@ -4323,7 +4377,7 @@
       <c r="A14" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B14" s="107" t="s">
+      <c r="B14" s="103" t="s">
         <v>76</v>
       </c>
       <c r="C14" s="59" t="s">
@@ -4337,7 +4391,7 @@
       <c r="A15" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="105"/>
+      <c r="B15" s="104"/>
       <c r="C15" s="59" t="s">
         <v>79</v>
       </c>
@@ -4349,7 +4403,7 @@
       <c r="A16" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B16" s="105"/>
+      <c r="B16" s="104"/>
       <c r="C16" s="59" t="s">
         <v>81</v>
       </c>
@@ -4361,7 +4415,7 @@
       <c r="A17" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="105"/>
+      <c r="B17" s="104"/>
       <c r="C17" s="59" t="s">
         <v>83</v>
       </c>
@@ -4373,7 +4427,7 @@
       <c r="A18" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B18" s="105"/>
+      <c r="B18" s="104"/>
       <c r="C18" s="59" t="s">
         <v>85</v>
       </c>
@@ -4385,7 +4439,7 @@
       <c r="A19" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="105"/>
+      <c r="B19" s="104"/>
       <c r="C19" s="59" t="s">
         <v>87</v>
       </c>
@@ -4397,7 +4451,7 @@
       <c r="A20" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="105"/>
+      <c r="B20" s="104"/>
       <c r="C20" s="59" t="s">
         <v>89</v>
       </c>
@@ -4409,7 +4463,7 @@
       <c r="A21" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="105"/>
+      <c r="B21" s="104"/>
       <c r="C21" s="59" t="s">
         <v>91</v>
       </c>
@@ -4421,7 +4475,7 @@
       <c r="A22" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B22" s="105"/>
+      <c r="B22" s="104"/>
       <c r="C22" s="59" t="s">
         <v>93</v>
       </c>
@@ -4448,7 +4502,7 @@
       <c r="A24" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="B24" s="107" t="s">
+      <c r="B24" s="103" t="s">
         <v>97</v>
       </c>
       <c r="C24" s="59" t="s">
@@ -4462,7 +4516,7 @@
       <c r="A25" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="B25" s="105"/>
+      <c r="B25" s="104"/>
       <c r="C25" s="59" t="s">
         <v>100</v>
       </c>
@@ -4474,7 +4528,7 @@
       <c r="A26" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="B26" s="105"/>
+      <c r="B26" s="104"/>
       <c r="C26" s="59" t="s">
         <v>102</v>
       </c>
@@ -4486,7 +4540,7 @@
       <c r="A27" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="B27" s="105"/>
+      <c r="B27" s="104"/>
       <c r="C27" s="59" t="s">
         <v>104</v>
       </c>
@@ -4498,7 +4552,7 @@
       <c r="A28" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="B28" s="105"/>
+      <c r="B28" s="104"/>
       <c r="C28" s="59" t="s">
         <v>106</v>
       </c>
@@ -4510,7 +4564,7 @@
       <c r="A29" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="B29" s="105"/>
+      <c r="B29" s="104"/>
       <c r="C29" s="59" t="s">
         <v>108</v>
       </c>
@@ -4522,7 +4576,7 @@
       <c r="A30" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="B30" s="105"/>
+      <c r="B30" s="104"/>
       <c r="C30" s="59" t="s">
         <v>70</v>
       </c>
@@ -4534,7 +4588,7 @@
       <c r="A31" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="B31" s="105"/>
+      <c r="B31" s="104"/>
       <c r="C31" s="59" t="s">
         <v>111</v>
       </c>
@@ -4561,7 +4615,7 @@
       <c r="A33" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="B33" s="107" t="s">
+      <c r="B33" s="103" t="s">
         <v>115</v>
       </c>
       <c r="C33" s="59" t="s">
@@ -4575,7 +4629,7 @@
       <c r="A34" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="B34" s="105"/>
+      <c r="B34" s="104"/>
       <c r="C34" s="59" t="s">
         <v>118</v>
       </c>
@@ -4587,7 +4641,7 @@
       <c r="A35" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="105"/>
+      <c r="B35" s="104"/>
       <c r="C35" s="59" t="s">
         <v>120</v>
       </c>
@@ -4599,7 +4653,7 @@
       <c r="A36" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="B36" s="105"/>
+      <c r="B36" s="104"/>
       <c r="C36" s="59" t="s">
         <v>122</v>
       </c>
@@ -4611,7 +4665,7 @@
       <c r="A37" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="B37" s="105"/>
+      <c r="B37" s="104"/>
       <c r="C37" s="59" t="s">
         <v>124</v>
       </c>
@@ -4623,7 +4677,7 @@
       <c r="A38" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="B38" s="105"/>
+      <c r="B38" s="104"/>
       <c r="C38" s="59" t="s">
         <v>126</v>
       </c>
@@ -4635,7 +4689,7 @@
       <c r="A39" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="B39" s="105"/>
+      <c r="B39" s="104"/>
       <c r="C39" s="59" t="s">
         <v>128</v>
       </c>
@@ -4647,7 +4701,7 @@
       <c r="A40" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="B40" s="105"/>
+      <c r="B40" s="104"/>
       <c r="C40" s="59" t="s">
         <v>130</v>
       </c>
@@ -4659,7 +4713,7 @@
       <c r="A41" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B41" s="105"/>
+      <c r="B41" s="104"/>
       <c r="C41" s="59" t="s">
         <v>132</v>
       </c>
@@ -4671,7 +4725,7 @@
       <c r="A42" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="B42" s="105"/>
+      <c r="B42" s="104"/>
       <c r="C42" s="59" t="s">
         <v>134</v>
       </c>
@@ -4683,7 +4737,7 @@
       <c r="A43" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="B43" s="105"/>
+      <c r="B43" s="104"/>
       <c r="C43" s="59" t="s">
         <v>136</v>
       </c>
@@ -4695,7 +4749,7 @@
       <c r="A44" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="B44" s="105"/>
+      <c r="B44" s="104"/>
       <c r="C44" s="59" t="s">
         <v>138</v>
       </c>
@@ -4707,7 +4761,7 @@
       <c r="A45" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="B45" s="105"/>
+      <c r="B45" s="104"/>
       <c r="C45" s="59" t="s">
         <v>140</v>
       </c>
@@ -4719,7 +4773,7 @@
       <c r="A46" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="B46" s="105"/>
+      <c r="B46" s="104"/>
       <c r="C46" s="59" t="s">
         <v>142</v>
       </c>
@@ -4731,7 +4785,7 @@
       <c r="A47" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="B47" s="105"/>
+      <c r="B47" s="104"/>
       <c r="C47" s="59" t="s">
         <v>144</v>
       </c>
@@ -4743,7 +4797,7 @@
       <c r="A48" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="B48" s="105"/>
+      <c r="B48" s="104"/>
       <c r="C48" s="59" t="s">
         <v>146</v>
       </c>
@@ -4755,7 +4809,7 @@
       <c r="A49" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="B49" s="105"/>
+      <c r="B49" s="104"/>
       <c r="C49" s="59" t="s">
         <v>148</v>
       </c>
@@ -4767,7 +4821,7 @@
       <c r="A50" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="B50" s="105"/>
+      <c r="B50" s="104"/>
       <c r="C50" s="59" t="s">
         <v>150</v>
       </c>
@@ -4779,7 +4833,7 @@
       <c r="A51" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="B51" s="105"/>
+      <c r="B51" s="104"/>
       <c r="C51" s="59" t="s">
         <v>152</v>
       </c>
@@ -4806,7 +4860,7 @@
       <c r="A53" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="B53" s="104" t="s">
+      <c r="B53" s="110" t="s">
         <v>156</v>
       </c>
       <c r="C53" s="59" t="s">
@@ -4820,7 +4874,7 @@
       <c r="A54" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="B54" s="105"/>
+      <c r="B54" s="104"/>
       <c r="C54" s="59" t="s">
         <v>159</v>
       </c>
@@ -4832,7 +4886,7 @@
       <c r="A55" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="B55" s="105"/>
+      <c r="B55" s="104"/>
       <c r="C55" s="59" t="s">
         <v>161</v>
       </c>
@@ -4859,7 +4913,7 @@
       <c r="A57" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="B57" s="107" t="s">
+      <c r="B57" s="103" t="s">
         <v>165</v>
       </c>
       <c r="C57" s="59" t="s">
@@ -4873,7 +4927,7 @@
       <c r="A58" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="B58" s="105"/>
+      <c r="B58" s="104"/>
       <c r="C58" s="59" t="s">
         <v>168</v>
       </c>
@@ -4900,7 +4954,7 @@
       <c r="A60" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="B60" s="107" t="s">
+      <c r="B60" s="103" t="s">
         <v>172</v>
       </c>
       <c r="C60" s="59" t="s">
@@ -4914,7 +4968,7 @@
       <c r="A61" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="B61" s="105"/>
+      <c r="B61" s="104"/>
       <c r="C61" s="59" t="s">
         <v>175</v>
       </c>
@@ -4926,7 +4980,7 @@
       <c r="A62" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="B62" s="105"/>
+      <c r="B62" s="104"/>
       <c r="C62" s="59" t="s">
         <v>177</v>
       </c>
@@ -4938,7 +4992,7 @@
       <c r="A63" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="B63" s="105"/>
+      <c r="B63" s="104"/>
       <c r="C63" s="59" t="s">
         <v>179</v>
       </c>
@@ -4950,7 +5004,7 @@
       <c r="A64" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="B64" s="105"/>
+      <c r="B64" s="104"/>
       <c r="C64" s="59" t="s">
         <v>181</v>
       </c>
@@ -4962,7 +5016,7 @@
       <c r="A65" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="B65" s="105"/>
+      <c r="B65" s="104"/>
       <c r="C65" s="59" t="s">
         <v>183</v>
       </c>
@@ -4974,7 +5028,7 @@
       <c r="A66" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="B66" s="105"/>
+      <c r="B66" s="104"/>
       <c r="C66" s="59" t="s">
         <v>185</v>
       </c>
@@ -4986,7 +5040,7 @@
       <c r="A67" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="B67" s="105"/>
+      <c r="B67" s="104"/>
       <c r="C67" s="59" t="s">
         <v>187</v>
       </c>
@@ -4998,7 +5052,7 @@
       <c r="A68" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="B68" s="105"/>
+      <c r="B68" s="104"/>
       <c r="C68" s="59" t="s">
         <v>189</v>
       </c>
@@ -5010,7 +5064,7 @@
       <c r="A69" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="B69" s="105"/>
+      <c r="B69" s="104"/>
       <c r="C69" s="59" t="s">
         <v>191</v>
       </c>
@@ -5022,7 +5076,7 @@
       <c r="A70" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="B70" s="105"/>
+      <c r="B70" s="104"/>
       <c r="C70" s="59" t="s">
         <v>193</v>
       </c>
@@ -5034,7 +5088,7 @@
       <c r="A71" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="B71" s="105"/>
+      <c r="B71" s="104"/>
       <c r="C71" s="59" t="s">
         <v>195</v>
       </c>
@@ -5046,7 +5100,7 @@
       <c r="A72" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="B72" s="105"/>
+      <c r="B72" s="104"/>
       <c r="C72" s="59" t="s">
         <v>197</v>
       </c>
@@ -5058,7 +5112,7 @@
       <c r="A73" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="B73" s="105"/>
+      <c r="B73" s="104"/>
       <c r="C73" s="59" t="s">
         <v>199</v>
       </c>
@@ -5070,7 +5124,7 @@
       <c r="A74" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="B74" s="105"/>
+      <c r="B74" s="104"/>
       <c r="C74" s="59" t="s">
         <v>201</v>
       </c>
@@ -5082,7 +5136,7 @@
       <c r="A75" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="B75" s="105"/>
+      <c r="B75" s="104"/>
       <c r="C75" s="59" t="s">
         <v>203</v>
       </c>
@@ -5109,7 +5163,7 @@
       <c r="A77" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="B77" s="104" t="s">
+      <c r="B77" s="110" t="s">
         <v>207</v>
       </c>
       <c r="C77" s="59" t="s">
@@ -5123,7 +5177,7 @@
       <c r="A78" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="B78" s="105"/>
+      <c r="B78" s="104"/>
       <c r="C78" s="59" t="s">
         <v>210</v>
       </c>
@@ -5135,7 +5189,7 @@
       <c r="A79" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="B79" s="105"/>
+      <c r="B79" s="104"/>
       <c r="C79" s="59" t="s">
         <v>212</v>
       </c>
@@ -5147,7 +5201,7 @@
       <c r="A80" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="B80" s="105"/>
+      <c r="B80" s="104"/>
       <c r="C80" s="59" t="s">
         <v>214</v>
       </c>
@@ -5159,7 +5213,7 @@
       <c r="A81" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="B81" s="105"/>
+      <c r="B81" s="104"/>
       <c r="C81" s="59" t="s">
         <v>216</v>
       </c>
@@ -5186,7 +5240,7 @@
       <c r="A83" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="B83" s="104" t="s">
+      <c r="B83" s="110" t="s">
         <v>220</v>
       </c>
       <c r="C83" s="59" t="s">
@@ -5200,7 +5254,7 @@
       <c r="A84" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="B84" s="105"/>
+      <c r="B84" s="104"/>
       <c r="C84" s="59" t="s">
         <v>223</v>
       </c>
@@ -5212,7 +5266,7 @@
       <c r="A85" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="B85" s="105"/>
+      <c r="B85" s="104"/>
       <c r="C85" s="59" t="s">
         <v>225</v>
       </c>
@@ -5224,7 +5278,7 @@
       <c r="A86" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="B86" s="105"/>
+      <c r="B86" s="104"/>
       <c r="C86" s="59" t="s">
         <v>227</v>
       </c>
@@ -5251,7 +5305,7 @@
       <c r="A88" s="12" t="s">
         <v>230</v>
       </c>
-      <c r="B88" s="104" t="s">
+      <c r="B88" s="110" t="s">
         <v>231</v>
       </c>
       <c r="C88" s="59" t="s">
@@ -5265,7 +5319,7 @@
       <c r="A89" s="12" t="s">
         <v>233</v>
       </c>
-      <c r="B89" s="105"/>
+      <c r="B89" s="104"/>
       <c r="C89" s="59" t="s">
         <v>234</v>
       </c>
@@ -5292,7 +5346,7 @@
       <c r="A91" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="B91" s="104" t="s">
+      <c r="B91" s="110" t="s">
         <v>238</v>
       </c>
       <c r="C91" s="59" t="s">
@@ -5306,7 +5360,7 @@
       <c r="A92" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="B92" s="105"/>
+      <c r="B92" s="104"/>
       <c r="C92" s="59" t="s">
         <v>241</v>
       </c>
@@ -5318,7 +5372,7 @@
       <c r="A93" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="B93" s="105"/>
+      <c r="B93" s="104"/>
       <c r="C93" s="59" t="s">
         <v>243</v>
       </c>
@@ -5330,7 +5384,7 @@
       <c r="A94" s="12" t="s">
         <v>244</v>
       </c>
-      <c r="B94" s="105"/>
+      <c r="B94" s="104"/>
       <c r="C94" s="59" t="s">
         <v>245</v>
       </c>
@@ -5342,7 +5396,7 @@
       <c r="A95" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="B95" s="105"/>
+      <c r="B95" s="104"/>
       <c r="C95" s="59" t="s">
         <v>247</v>
       </c>
@@ -5354,7 +5408,7 @@
       <c r="A96" s="12" t="s">
         <v>248</v>
       </c>
-      <c r="B96" s="105"/>
+      <c r="B96" s="104"/>
       <c r="C96" s="59" t="s">
         <v>249</v>
       </c>
@@ -5366,7 +5420,7 @@
       <c r="A97" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="B97" s="105"/>
+      <c r="B97" s="104"/>
       <c r="C97" s="59" t="s">
         <v>251</v>
       </c>
@@ -5407,10 +5461,10 @@
     <row r="101" spans="1:6">
       <c r="A101" s="12"/>
       <c r="B101" s="64"/>
-      <c r="C101" s="106" t="s">
+      <c r="C101" s="111" t="s">
         <v>255</v>
       </c>
-      <c r="D101" s="106"/>
+      <c r="D101" s="111"/>
       <c r="E101" s="60"/>
       <c r="F101" s="53"/>
     </row>
@@ -5453,12 +5507,6 @@
   <sheetProtection algorithmName="SHA-512" hashValue="InmqKlhhVhE+dGbIYDiSRnLE+IlAZxdLfnctzqDZDARVCn6iziD6wICeby41lmvE4W1J88KUyAnY0y7x+sw6lQ==" saltValue="K8srq741x0YFfj6gj3u+2g==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="14">
-    <mergeCell ref="B33:B51"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B14:B22"/>
-    <mergeCell ref="B24:B31"/>
     <mergeCell ref="B91:B97"/>
     <mergeCell ref="C101:D101"/>
     <mergeCell ref="B53:B55"/>
@@ -5467,6 +5515,12 @@
     <mergeCell ref="B77:B81"/>
     <mergeCell ref="B83:B86"/>
     <mergeCell ref="B88:B89"/>
+    <mergeCell ref="B33:B51"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B14:B22"/>
+    <mergeCell ref="B24:B31"/>
   </mergeCells>
   <conditionalFormatting sqref="B23">
     <cfRule type="expression" dxfId="13" priority="13">
@@ -5586,32 +5640,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="68" t="s">
         <v>260</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="68" t="s">
         <v>261</v>
       </c>
-      <c r="C1" s="70" t="s">
+      <c r="C1" s="69" t="s">
         <v>262</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="68" t="s">
         <v>260</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="F1" s="68" t="s">
         <v>261</v>
       </c>
-      <c r="G1" s="70" t="s">
+      <c r="G1" s="69" t="s">
         <v>262</v>
       </c>
-      <c r="H1" s="70"/>
-      <c r="I1" s="69" t="s">
+      <c r="H1" s="69"/>
+      <c r="I1" s="68" t="s">
         <v>260</v>
       </c>
-      <c r="J1" s="69" t="s">
+      <c r="J1" s="68" t="s">
         <v>261</v>
       </c>
-      <c r="K1" s="70" t="s">
+      <c r="K1" s="69" t="s">
         <v>262</v>
       </c>
       <c r="M1" t="s">
@@ -5625,7 +5679,7 @@
       <c r="B2" t="s">
         <v>264</v>
       </c>
-      <c r="C2" s="71">
+      <c r="C2" s="70">
         <v>1</v>
       </c>
       <c r="E2" t="s">
@@ -5634,7 +5688,7 @@
       <c r="F2" t="s">
         <v>265</v>
       </c>
-      <c r="G2" s="72">
+      <c r="G2" s="71">
         <v>2</v>
       </c>
       <c r="I2" t="s">
@@ -5657,7 +5711,7 @@
       <c r="B3" t="s">
         <v>269</v>
       </c>
-      <c r="C3" s="71">
+      <c r="C3" s="70">
         <v>1</v>
       </c>
       <c r="E3" t="s">
@@ -5666,7 +5720,7 @@
       <c r="F3" t="s">
         <v>271</v>
       </c>
-      <c r="G3" s="72">
+      <c r="G3" s="71">
         <v>2</v>
       </c>
       <c r="I3" t="s">
@@ -5689,7 +5743,7 @@
       <c r="B4" t="s">
         <v>275</v>
       </c>
-      <c r="C4" s="71">
+      <c r="C4" s="70">
         <v>1</v>
       </c>
       <c r="E4" t="s">
@@ -5698,7 +5752,7 @@
       <c r="F4" t="s">
         <v>277</v>
       </c>
-      <c r="G4" s="72">
+      <c r="G4" s="71">
         <v>2</v>
       </c>
       <c r="I4" t="s">
@@ -5718,7 +5772,7 @@
       <c r="B5" t="s">
         <v>281</v>
       </c>
-      <c r="C5" s="71">
+      <c r="C5" s="70">
         <v>1</v>
       </c>
       <c r="E5" t="s">
@@ -5727,7 +5781,7 @@
       <c r="F5" t="s">
         <v>282</v>
       </c>
-      <c r="G5" s="72">
+      <c r="G5" s="71">
         <v>2</v>
       </c>
       <c r="I5" t="s">
@@ -5747,7 +5801,7 @@
       <c r="B6" t="s">
         <v>286</v>
       </c>
-      <c r="C6" s="71">
+      <c r="C6" s="70">
         <v>1</v>
       </c>
       <c r="E6" t="s">
@@ -5756,7 +5810,7 @@
       <c r="F6" t="s">
         <v>287</v>
       </c>
-      <c r="G6" s="72">
+      <c r="G6" s="71">
         <v>2</v>
       </c>
       <c r="I6" t="s">
@@ -5773,7 +5827,7 @@
       <c r="B7" t="s">
         <v>290</v>
       </c>
-      <c r="C7" s="71">
+      <c r="C7" s="70">
         <v>1</v>
       </c>
       <c r="E7" t="s">
@@ -5782,7 +5836,7 @@
       <c r="F7" t="s">
         <v>291</v>
       </c>
-      <c r="G7" s="72">
+      <c r="G7" s="71">
         <v>2</v>
       </c>
       <c r="I7" t="s">
@@ -5799,7 +5853,7 @@
       <c r="B8" t="s">
         <v>294</v>
       </c>
-      <c r="C8" s="71">
+      <c r="C8" s="70">
         <v>1</v>
       </c>
       <c r="E8" t="s">
@@ -5808,7 +5862,7 @@
       <c r="F8" t="s">
         <v>295</v>
       </c>
-      <c r="G8" s="72">
+      <c r="G8" s="71">
         <v>2</v>
       </c>
       <c r="I8" t="s">
@@ -5825,7 +5879,7 @@
       <c r="B9" t="s">
         <v>297</v>
       </c>
-      <c r="C9" s="71">
+      <c r="C9" s="70">
         <v>1</v>
       </c>
       <c r="E9" t="s">
@@ -5834,7 +5888,7 @@
       <c r="F9" t="s">
         <v>299</v>
       </c>
-      <c r="G9" s="72">
+      <c r="G9" s="71">
         <v>2</v>
       </c>
     </row>
@@ -5845,7 +5899,7 @@
       <c r="B10" t="s">
         <v>301</v>
       </c>
-      <c r="C10" s="71">
+      <c r="C10" s="70">
         <v>1</v>
       </c>
       <c r="E10" t="s">
@@ -5854,7 +5908,7 @@
       <c r="F10" t="s">
         <v>302</v>
       </c>
-      <c r="G10" s="72">
+      <c r="G10" s="71">
         <v>2</v>
       </c>
     </row>
@@ -5865,7 +5919,7 @@
       <c r="B11" t="s">
         <v>304</v>
       </c>
-      <c r="C11" s="71">
+      <c r="C11" s="70">
         <v>1</v>
       </c>
       <c r="E11" t="s">
@@ -5874,7 +5928,7 @@
       <c r="F11" t="s">
         <v>305</v>
       </c>
-      <c r="G11" s="72">
+      <c r="G11" s="71">
         <v>2</v>
       </c>
     </row>
@@ -5885,7 +5939,7 @@
       <c r="B12" t="s">
         <v>307</v>
       </c>
-      <c r="C12" s="71">
+      <c r="C12" s="70">
         <v>1</v>
       </c>
       <c r="E12" t="s">
@@ -5894,7 +5948,7 @@
       <c r="F12" t="s">
         <v>308</v>
       </c>
-      <c r="G12" s="72">
+      <c r="G12" s="71">
         <v>2</v>
       </c>
     </row>
@@ -5905,7 +5959,7 @@
       <c r="B13" t="s">
         <v>310</v>
       </c>
-      <c r="C13" s="71">
+      <c r="C13" s="70">
         <v>1</v>
       </c>
       <c r="E13" t="s">
@@ -5914,7 +5968,7 @@
       <c r="F13" t="s">
         <v>312</v>
       </c>
-      <c r="G13" s="72">
+      <c r="G13" s="71">
         <v>2</v>
       </c>
     </row>
@@ -5925,7 +5979,7 @@
       <c r="B14" t="s">
         <v>314</v>
       </c>
-      <c r="C14" s="71">
+      <c r="C14" s="70">
         <v>1</v>
       </c>
       <c r="E14" t="s">
@@ -5934,7 +5988,7 @@
       <c r="F14" t="s">
         <v>316</v>
       </c>
-      <c r="G14" s="72">
+      <c r="G14" s="71">
         <v>2</v>
       </c>
     </row>
@@ -5945,7 +5999,7 @@
       <c r="B15" t="s">
         <v>318</v>
       </c>
-      <c r="C15" s="71">
+      <c r="C15" s="70">
         <v>1</v>
       </c>
       <c r="E15" t="s">
@@ -5954,7 +6008,7 @@
       <c r="F15" t="s">
         <v>320</v>
       </c>
-      <c r="G15" s="72">
+      <c r="G15" s="71">
         <v>2</v>
       </c>
     </row>
@@ -5965,7 +6019,7 @@
       <c r="B16" t="s">
         <v>322</v>
       </c>
-      <c r="C16" s="71">
+      <c r="C16" s="70">
         <v>1</v>
       </c>
       <c r="E16" t="s">
@@ -5974,7 +6028,7 @@
       <c r="F16" t="s">
         <v>324</v>
       </c>
-      <c r="G16" s="72">
+      <c r="G16" s="71">
         <v>2</v>
       </c>
     </row>
@@ -5985,7 +6039,7 @@
       <c r="B17" t="s">
         <v>326</v>
       </c>
-      <c r="C17" s="71">
+      <c r="C17" s="70">
         <v>1</v>
       </c>
       <c r="E17" t="s">
@@ -5994,7 +6048,7 @@
       <c r="F17" t="s">
         <v>328</v>
       </c>
-      <c r="G17" s="72">
+      <c r="G17" s="71">
         <v>2</v>
       </c>
     </row>
@@ -6005,7 +6059,7 @@
       <c r="B18" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="71">
+      <c r="C18" s="70">
         <v>1</v>
       </c>
       <c r="E18" t="s">
@@ -6014,7 +6068,7 @@
       <c r="F18" t="s">
         <v>331</v>
       </c>
-      <c r="G18" s="72">
+      <c r="G18" s="71">
         <v>2</v>
       </c>
     </row>
@@ -6025,7 +6079,7 @@
       <c r="B19" t="s">
         <v>165</v>
       </c>
-      <c r="C19" s="71">
+      <c r="C19" s="70">
         <v>1</v>
       </c>
       <c r="E19" t="s">
@@ -6034,7 +6088,7 @@
       <c r="F19" t="s">
         <v>334</v>
       </c>
-      <c r="G19" s="72">
+      <c r="G19" s="71">
         <v>2</v>
       </c>
     </row>
@@ -6045,7 +6099,7 @@
       <c r="B20" t="s">
         <v>207</v>
       </c>
-      <c r="C20" s="71">
+      <c r="C20" s="70">
         <v>1</v>
       </c>
       <c r="E20" t="s">
@@ -6054,7 +6108,7 @@
       <c r="F20" t="s">
         <v>336</v>
       </c>
-      <c r="G20" s="72">
+      <c r="G20" s="71">
         <v>2</v>
       </c>
     </row>
@@ -6065,7 +6119,7 @@
       <c r="B21" t="s">
         <v>220</v>
       </c>
-      <c r="C21" s="71">
+      <c r="C21" s="70">
         <v>1</v>
       </c>
       <c r="E21" t="s">
@@ -6074,7 +6128,7 @@
       <c r="F21" t="s">
         <v>338</v>
       </c>
-      <c r="G21" s="72">
+      <c r="G21" s="71">
         <v>2</v>
       </c>
     </row>
@@ -6085,7 +6139,7 @@
       <c r="B22" t="s">
         <v>340</v>
       </c>
-      <c r="C22" s="71">
+      <c r="C22" s="70">
         <v>1</v>
       </c>
       <c r="E22" t="s">
@@ -6094,7 +6148,7 @@
       <c r="F22" t="s">
         <v>342</v>
       </c>
-      <c r="G22" s="72">
+      <c r="G22" s="71">
         <v>2</v>
       </c>
     </row>
@@ -6105,7 +6159,7 @@
       <c r="B23" t="s">
         <v>344</v>
       </c>
-      <c r="C23" s="71">
+      <c r="C23" s="70">
         <v>1</v>
       </c>
     </row>
@@ -6116,7 +6170,7 @@
       <c r="B24" t="s">
         <v>346</v>
       </c>
-      <c r="C24" s="71">
+      <c r="C24" s="70">
         <v>1</v>
       </c>
     </row>
@@ -6127,7 +6181,7 @@
       <c r="B25" t="s">
         <v>348</v>
       </c>
-      <c r="C25" s="71">
+      <c r="C25" s="70">
         <v>1</v>
       </c>
     </row>
@@ -6138,7 +6192,7 @@
       <c r="B26" t="s">
         <v>350</v>
       </c>
-      <c r="C26" s="71">
+      <c r="C26" s="70">
         <v>1</v>
       </c>
     </row>
@@ -6149,7 +6203,7 @@
       <c r="B27" t="s">
         <v>352</v>
       </c>
-      <c r="C27" s="71">
+      <c r="C27" s="70">
         <v>1</v>
       </c>
     </row>
@@ -6217,10 +6271,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="29"/>
-      <c r="F4" s="113" t="s">
+      <c r="F4" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="114"/>
+      <c r="G4" s="116"/>
       <c r="H4" s="1">
         <v>208</v>
       </c>
@@ -6229,10 +6283,10 @@
       </c>
     </row>
     <row r="5" spans="2:10" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1">
-      <c r="F5" s="115" t="s">
+      <c r="F5" s="117" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="116"/>
+      <c r="G5" s="118"/>
       <c r="H5" s="42">
         <v>8</v>
       </c>
@@ -6245,7 +6299,7 @@
       <c r="G6" s="40"/>
     </row>
     <row r="7" spans="2:10" ht="70" customHeight="1">
-      <c r="B7" s="117" t="s">
+      <c r="B7" s="112" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="19" t="s">
@@ -6263,8 +6317,8 @@
       <c r="J7"/>
     </row>
     <row r="8" spans="2:10" ht="26" customHeight="1">
-      <c r="B8" s="118"/>
-      <c r="H8" s="121"/>
+      <c r="B8" s="113"/>
+      <c r="H8" s="114"/>
       <c r="J8"/>
     </row>
     <row r="9" spans="2:10" ht="38.25" customHeight="1">
@@ -6301,7 +6355,7 @@
       <c r="J11"/>
     </row>
     <row r="12" spans="2:10" ht="69" customHeight="1">
-      <c r="B12" s="117" t="s">
+      <c r="B12" s="112" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="37" t="s">
@@ -6316,11 +6370,11 @@
       <c r="J12"/>
     </row>
     <row r="13" spans="2:10" ht="34.5" customHeight="1">
-      <c r="B13" s="118"/>
+      <c r="B13" s="113"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="9"/>
-      <c r="G13" s="121" t="s">
+      <c r="G13" s="114" t="s">
         <v>21</v>
       </c>
       <c r="J13"/>
@@ -6334,7 +6388,7 @@
       <c r="E14" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="121"/>
+      <c r="G14" s="114"/>
     </row>
     <row r="15" spans="2:10" s="3" customFormat="1" ht="6.75" customHeight="1">
       <c r="B15" s="17"/>
@@ -6378,19 +6432,49 @@
       <c r="D19" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="nQ8joA74Rsh2Kx3Wfl1MFY2uo8GlElYBj87kqHVIo37r55P2tUu/gqoh5+2Pc6vWI/gF3F4U69Fb3n3B58JSQQ==" saltValue="TyXrh0FDS1+0gOHNSzrziQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="UPLbUm1+bqbfXmnMLcE8Rn9CI/NBcf5Up43OtNldliMyg6/LXkybQr77PYuL6n+coy8Bh+riYhCBrKUx4lshFg==" saltValue="IIHMr8JbSN/brD69Lfg/dg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="7">
+    <mergeCell ref="H7:H8"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="E7:F7"/>
-    <mergeCell ref="H7:H8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A347A571-7E1E-DF47-8068-65B08AC7DB39}">
+          <x14:formula1>
+            <xm:f>Listes!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>E9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EF1F3728-9960-744D-9924-771E6AEB79B6}">
+          <x14:formula1>
+            <xm:f>Listes!$C$2:$C$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>F9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9C810209-D42A-4D41-BE16-7090B008B727}">
+          <x14:formula1>
+            <xm:f>Listes!$A$9:$A$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>E14</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{72E23789-0823-1C41-90D4-0C8B73716399}">
+          <x14:formula1>
+            <xm:f>Listes!$C$9:$C$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>E16</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6399,7 +6483,7 @@
   <dimension ref="B1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6435,12 +6519,12 @@
         <v>1</v>
       </c>
       <c r="D3" s="28"/>
-      <c r="F3" s="122" t="s">
+      <c r="F3" s="121" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="123"/>
-      <c r="H3" s="123"/>
-      <c r="I3" s="124"/>
+      <c r="G3" s="122"/>
+      <c r="H3" s="122"/>
+      <c r="I3" s="123"/>
       <c r="J3"/>
     </row>
     <row r="4" spans="2:10" s="3" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
@@ -6449,10 +6533,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="29"/>
-      <c r="F4" s="113" t="s">
+      <c r="F4" s="115" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="114"/>
+      <c r="G4" s="116"/>
       <c r="H4" s="1">
         <v>1607</v>
       </c>
@@ -6461,10 +6545,10 @@
       </c>
     </row>
     <row r="5" spans="2:10" s="3" customFormat="1" ht="24.75" customHeight="1" thickBot="1">
-      <c r="F5" s="115" t="s">
+      <c r="F5" s="117" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="116"/>
+      <c r="G5" s="118"/>
       <c r="H5" s="39">
         <v>35</v>
       </c>
@@ -6479,7 +6563,7 @@
       </c>
     </row>
     <row r="7" spans="2:10" ht="70" customHeight="1">
-      <c r="B7" s="117" t="s">
+      <c r="B7" s="112" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="19" t="s">
@@ -6497,8 +6581,8 @@
       <c r="J7"/>
     </row>
     <row r="8" spans="2:10" ht="26" customHeight="1">
-      <c r="B8" s="118"/>
-      <c r="H8" s="121"/>
+      <c r="B8" s="113"/>
+      <c r="H8" s="114"/>
       <c r="J8"/>
     </row>
     <row r="9" spans="2:10" ht="38.25" customHeight="1">
@@ -6535,7 +6619,7 @@
       <c r="J11"/>
     </row>
     <row r="12" spans="2:10" ht="69" customHeight="1">
-      <c r="B12" s="117" t="s">
+      <c r="B12" s="112" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="37" t="s">
@@ -6550,11 +6634,11 @@
       <c r="J12"/>
     </row>
     <row r="13" spans="2:10" ht="34.5" customHeight="1">
-      <c r="B13" s="118"/>
+      <c r="B13" s="113"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="9"/>
-      <c r="G13" s="121" t="s">
+      <c r="G13" s="114" t="s">
         <v>21</v>
       </c>
       <c r="J13"/>
@@ -6568,7 +6652,7 @@
       <c r="E14" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="121"/>
+      <c r="G14" s="114"/>
     </row>
     <row r="15" spans="2:10" s="3" customFormat="1" ht="6.75" customHeight="1">
       <c r="B15" s="17"/>
@@ -6612,7 +6696,7 @@
       <c r="D19" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="xRHkrPVKkhuRjV5u2xVaW4HZXUe0clHppbAfBQ5iIJFNEE4Gbw4lYoNTH/CilznojGL+pTtz514JcRKZOgFmhg==" saltValue="2QeW7OiIyb8W0A7ku4nALg==" spinCount="100000" sheet="1" objects="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="3niYrB0o6qf6v+PSHMrO4Z/NUX5mRFNdVO+Yrc0OkSXoAXux8c7HqMx5VlRPv+WUh+Y9LCyMSAHO8F9VRIQvtQ==" saltValue="MHmavSrorJTb/4/9UqPOLA==" spinCount="100000" sheet="1" objects="1" selectLockedCells="1"/>
   <mergeCells count="8">
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="G13:G14"/>
@@ -6626,6 +6710,24 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3201A92A-2B0E-DF4D-A144-FE357CD3D3CD}">
+          <x14:formula1>
+            <xm:f>Listes!$A$9:$A$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>E9 E14</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{728CCD2B-3897-E247-BA89-46FF984E318E}">
+          <x14:formula1>
+            <xm:f>Listes!$C$9:$C$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>F9 E16</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6644,7 +6746,7 @@
     <col min="3" max="3" width="43.5" style="46" customWidth="1"/>
     <col min="4" max="4" width="9" style="3" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" style="12" customWidth="1"/>
-    <col min="6" max="6" width="4" style="79" customWidth="1"/>
+    <col min="6" max="6" width="4" style="78" customWidth="1"/>
     <col min="7" max="7" width="6.6640625" style="3" customWidth="1"/>
     <col min="8" max="8" width="11.33203125" style="3"/>
     <col min="9" max="9" width="22.33203125" style="3" customWidth="1"/>
@@ -6657,32 +6759,32 @@
       <c r="F1" s="3"/>
     </row>
     <row r="2" spans="3:9" ht="54.75" customHeight="1">
-      <c r="C2" s="125" t="s">
+      <c r="C2" s="124" t="s">
         <v>355</v>
       </c>
-      <c r="D2" s="125"/>
-      <c r="E2" s="125"/>
-      <c r="F2" s="125"/>
-      <c r="G2" s="125"/>
-      <c r="H2" s="125"/>
-      <c r="I2" s="125"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="124"/>
+      <c r="F2" s="124"/>
+      <c r="G2" s="124"/>
+      <c r="H2" s="124"/>
+      <c r="I2" s="124"/>
     </row>
     <row r="3" spans="3:9" ht="27.75" customHeight="1">
       <c r="C3" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="126" t="s">
+      <c r="D3" s="125" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="127"/>
-      <c r="G3" s="128" t="s">
+      <c r="E3" s="126"/>
+      <c r="G3" s="127" t="s">
         <v>356</v>
       </c>
-      <c r="H3" s="128"/>
-      <c r="I3" s="128"/>
+      <c r="H3" s="127"/>
+      <c r="I3" s="127"/>
     </row>
     <row r="4" spans="3:9" ht="23.25" customHeight="1">
-      <c r="C4" s="80" t="s">
+      <c r="C4" s="79" t="s">
         <v>357</v>
       </c>
       <c r="D4" s="43" t="str">
@@ -6691,14 +6793,14 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="53"/>
-      <c r="G4" s="79"/>
+      <c r="G4" s="78"/>
     </row>
     <row r="5" spans="3:9" ht="7.5" customHeight="1">
       <c r="C5" s="47"/>
       <c r="D5" s="43"/>
       <c r="E5" s="3"/>
       <c r="F5" s="12"/>
-      <c r="G5" s="79"/>
+      <c r="G5" s="78"/>
     </row>
     <row r="6" spans="3:9" ht="23.25" customHeight="1">
       <c r="C6" s="47" t="s">
@@ -6709,20 +6811,20 @@
         <v>42</v>
       </c>
       <c r="F6" s="12"/>
-      <c r="G6" s="79"/>
-      <c r="H6" s="81"/>
-      <c r="I6" s="81"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="80"/>
+      <c r="I6" s="80"/>
     </row>
     <row r="7" spans="3:9" ht="25.25" customHeight="1">
       <c r="C7" s="47"/>
-      <c r="D7" s="82" t="s">
+      <c r="D7" s="81" t="s">
         <v>358</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="12"/>
-      <c r="G7" s="83"/>
-      <c r="H7" s="81"/>
-      <c r="I7" s="81"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="80"/>
     </row>
     <row r="8" spans="3:9" ht="24" customHeight="1">
       <c r="C8" s="47" t="s">
@@ -6733,20 +6835,20 @@
         <v>44</v>
       </c>
       <c r="F8" s="12"/>
-      <c r="G8" s="79"/>
-      <c r="H8" s="81"/>
-      <c r="I8" s="81"/>
+      <c r="G8" s="78"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="80"/>
     </row>
     <row r="9" spans="3:9" ht="18" customHeight="1">
       <c r="C9" s="47"/>
-      <c r="D9" s="84" t="s">
+      <c r="D9" s="83" t="s">
         <v>359</v>
       </c>
       <c r="E9" s="48"/>
       <c r="F9" s="12"/>
-      <c r="G9" s="79"/>
-      <c r="H9" s="81"/>
-      <c r="I9" s="81"/>
+      <c r="G9" s="78"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="80"/>
     </row>
     <row r="10" spans="3:9" ht="36" customHeight="1">
       <c r="C10" s="47"/>
@@ -6755,33 +6857,33 @@
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="3:9" ht="24" customHeight="1">
-      <c r="C11" s="85" t="s">
+      <c r="C11" s="84" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="86">
+      <c r="D11" s="85">
         <f>IF(D3="MAGISTRAT",D6*D8*[1]Listes!D3,D6*D8*[1]Fonctionnaires!H4/7)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="87" t="s">
+      <c r="E11" s="86" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="88" t="s">
+      <c r="F11" s="87" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="89">
+      <c r="G11" s="88">
         <f>IF(D3="FONCTIONNAIRE",D11*7,D11*8)</f>
         <v>0</v>
       </c>
-      <c r="H11" s="87" t="s">
+      <c r="H11" s="86" t="s">
         <v>46</v>
       </c>
-      <c r="I11" s="90"/>
+      <c r="I11" s="89"/>
     </row>
     <row r="12" spans="3:9" ht="24" customHeight="1">
-      <c r="C12" s="91" t="s">
+      <c r="C12" s="90" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="92">
+      <c r="D12" s="91">
         <f>D11/12</f>
         <v>0</v>
       </c>
@@ -6791,59 +6893,59 @@
       <c r="F12" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="93">
+      <c r="G12" s="92">
         <f>IF(D4="FONCTIONNAIRE",D12*7,D12*8)</f>
         <v>0</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="I12" s="94"/>
+      <c r="I12" s="93"/>
     </row>
     <row r="13" spans="3:9" ht="24" customHeight="1">
-      <c r="C13" s="95" t="s">
+      <c r="C13" s="94" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="96">
+      <c r="D13" s="95">
         <f>(D8*D6)*5</f>
         <v>0</v>
       </c>
-      <c r="E13" s="97" t="s">
+      <c r="E13" s="96" t="s">
         <v>362</v>
       </c>
-      <c r="F13" s="98" t="s">
+      <c r="F13" s="97" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="99">
+      <c r="G13" s="98">
         <f>IF(D3="FONCTIONNAIRE",D13*7,D13*8)</f>
         <v>0</v>
       </c>
-      <c r="H13" s="97" t="s">
+      <c r="H13" s="96" t="s">
         <v>363</v>
       </c>
-      <c r="I13" s="100"/>
+      <c r="I13" s="99"/>
     </row>
     <row r="14" spans="3:9" ht="16.25" customHeight="1">
-      <c r="C14" s="101" t="s">
+      <c r="C14" s="100" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="15" spans="3:9" ht="16.25" customHeight="1">
-      <c r="C15" s="101" t="s">
+      <c r="C15" s="100" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="16" spans="3:9" ht="24" customHeight="1">
-      <c r="C16" s="102"/>
+      <c r="C16" s="101"/>
     </row>
     <row r="17" spans="3:3" ht="24" customHeight="1">
-      <c r="C17" s="103"/>
+      <c r="C17" s="102"/>
     </row>
     <row r="18" spans="3:3" ht="24" customHeight="1">
-      <c r="C18" s="102"/>
+      <c r="C18" s="101"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Gy5QNriGlaVHeAjPum4cM0C4+yAHxmDli0jwulpHKqegGEbXID+fQiRrC1N4zJrSKGFxFCw3CH18lQT24sk6Nw==" saltValue="wVeS2Y8bMsGjmNDXNpg93A==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="aDXNkJ2efhryHHrInatlkZ3y7C07jmVd4jT9/If0kG3duKVA++0b+Qvz89QqdJ++xH35TQ5tb2xjeV5Kx2n8iQ==" saltValue="KteL1vZhNZpNVuhiO2P9Vg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="3">
     <mergeCell ref="C2:I2"/>
     <mergeCell ref="D3:E3"/>
@@ -6852,6 +6954,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C7FF2140-AB7E-834C-8562-FC8C1D3491A0}">
+          <x14:formula1>
+            <xm:f>Listes!$A$15:$A$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3:E3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6860,7 +6974,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6892,6 +7006,7 @@
         <v>27</v>
       </c>
       <c r="D3">
+        <f>[2]Magistrats!H4</f>
         <v>208</v>
       </c>
       <c r="F3" t="s">
@@ -6918,6 +7033,7 @@
         <v>2</v>
       </c>
       <c r="B5">
+        <f>1/[2]Magistrats!H5</f>
         <v>0.125</v>
       </c>
       <c r="C5" t="s">
@@ -6955,12 +7071,14 @@
         <v>1</v>
       </c>
       <c r="B10" s="38">
+        <f>[2]Fonctionnaires!H5/5</f>
         <v>7</v>
       </c>
       <c r="C10" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="38">
+        <f>[2]Fonctionnaires!H4/[2]Listes!B10</f>
         <v>229.57142857142858</v>
       </c>
     </row>
@@ -6976,6 +7094,7 @@
         <v>28</v>
       </c>
       <c r="D11" s="38">
+        <f>[2]Fonctionnaires!H4/[2]Fonctionnaires!H5</f>
         <v>45.914285714285711</v>
       </c>
     </row>
@@ -7003,13 +7122,18 @@
         <v>1</v>
       </c>
     </row>
+    <row r="15" spans="1:6" ht="16">
+      <c r="A15" s="128" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="16" spans="1:6" ht="16">
-      <c r="A16" s="68" t="s">
-        <v>50</v>
+      <c r="A16" s="128" t="s">
+        <v>366</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="ylOsT+Xc0ZF6Rv8Nx2hLJ1LRk4ihR/orFjBlyZjUAIQ86qwXmN9RREU9VYXYrHTBKxNZ9Pj6lIQKB4AZRUecnw==" saltValue="s31b1g37+oO1Eckh4qZr8Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="c5QCgm2ESz3VOddRZLTYqWb5+a9so9ILN4xf/GmfxgwN3ZV9BtrxO/pa0N9vUUk3XfkCvDQ1nTgxUTpz5z0u/Q==" saltValue="qcV35N0E7yxKjOYV+OK3SQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix excel fiche agent
</commit_message>
<xml_diff>
--- a/front/src/assets/Fiche_agent_template.xlsx
+++ b/front/src/assets/Fiche_agent_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693CACA0-2F1C-2A41-8590-67A7584D1189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C618D1D1-4246-DD49-8763-C58BF0B6AA7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17840" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
   </bookViews>
@@ -22,7 +22,6 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId7"/>
-    <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Fonction!$A$1:$C$27</definedName>
@@ -1734,7 +1733,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1993,9 +1992,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -2029,10 +2025,17 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="12" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="4" fontId="12" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2052,11 +2055,11 @@
     <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="12" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2064,9 +2067,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -2081,9 +2081,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2108,7 +2105,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Milliers" xfId="2" builtinId="3"/>
@@ -3694,151 +3690,6 @@
       <sheetName val="Listes"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="4">
-          <cell r="H4">
-            <v>1607</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>unités</v>
-          </cell>
-          <cell r="C2" t="str">
-            <v>fréquence</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>jours</v>
-          </cell>
-          <cell r="B3">
-            <v>1</v>
-          </cell>
-          <cell r="C3" t="str">
-            <v>par jour</v>
-          </cell>
-          <cell r="D3">
-            <v>208</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>demi-journées</v>
-          </cell>
-          <cell r="B4">
-            <v>0.5</v>
-          </cell>
-          <cell r="C4" t="str">
-            <v>par semaine</v>
-          </cell>
-          <cell r="D4">
-            <v>41.6</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>heures</v>
-          </cell>
-          <cell r="B5">
-            <v>0.125</v>
-          </cell>
-          <cell r="C5" t="str">
-            <v>par mois</v>
-          </cell>
-          <cell r="D5">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="C6" t="str">
-            <v>par an</v>
-          </cell>
-          <cell r="D6">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>unités</v>
-          </cell>
-          <cell r="C9" t="str">
-            <v>fréquence</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>jours</v>
-          </cell>
-          <cell r="B10">
-            <v>7</v>
-          </cell>
-          <cell r="C10" t="str">
-            <v>par jour</v>
-          </cell>
-          <cell r="D10">
-            <v>229.57142857142858</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>demi-journées</v>
-          </cell>
-          <cell r="B11">
-            <v>3.5</v>
-          </cell>
-          <cell r="C11" t="str">
-            <v>par semaine</v>
-          </cell>
-          <cell r="D11">
-            <v>45.914285714285711</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>heures</v>
-          </cell>
-          <cell r="B12">
-            <v>1</v>
-          </cell>
-          <cell r="C12" t="str">
-            <v>par mois</v>
-          </cell>
-          <cell r="D12">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="C13" t="str">
-            <v>par an</v>
-          </cell>
-          <cell r="D13">
-            <v>1</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Magistrats"/>
-      <sheetName val="Fonctionnaires"/>
-      <sheetName val="Reconvertir un pourcentage"/>
-      <sheetName val="Listes"/>
-    </sheetNames>
-    <sheetDataSet>
       <sheetData sheetId="0">
         <row r="4">
           <cell r="H4">
@@ -4271,12 +4122,12 @@
     </row>
     <row r="6" spans="1:7" ht="56" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="50"/>
-      <c r="B6" s="105" t="s">
+      <c r="B6" s="107" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="105"/>
-      <c r="D6" s="105"/>
-      <c r="E6" s="106"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="108"/>
       <c r="F6" s="53"/>
     </row>
     <row r="7" spans="1:7" ht="110" customHeight="1" thickTop="1">
@@ -4301,8 +4152,8 @@
       <c r="B8" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="107"/>
-      <c r="D8" s="108"/>
+      <c r="C8" s="109"/>
+      <c r="D8" s="110"/>
       <c r="E8" s="73" t="s">
         <v>63</v>
       </c>
@@ -4312,7 +4163,7 @@
       <c r="A9" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="109" t="s">
+      <c r="B9" s="111" t="s">
         <v>65</v>
       </c>
       <c r="C9" s="59" t="s">
@@ -4326,7 +4177,7 @@
       <c r="A10" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="109"/>
+      <c r="B10" s="111"/>
       <c r="C10" s="59" t="s">
         <v>68</v>
       </c>
@@ -4338,7 +4189,7 @@
       <c r="A11" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="109"/>
+      <c r="B11" s="111"/>
       <c r="C11" s="59" t="s">
         <v>70</v>
       </c>
@@ -4350,7 +4201,7 @@
       <c r="A12" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="109"/>
+      <c r="B12" s="111"/>
       <c r="C12" s="59" t="s">
         <v>72</v>
       </c>
@@ -4377,7 +4228,7 @@
       <c r="A14" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B14" s="103" t="s">
+      <c r="B14" s="106" t="s">
         <v>76</v>
       </c>
       <c r="C14" s="59" t="s">
@@ -4502,7 +4353,7 @@
       <c r="A24" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="B24" s="103" t="s">
+      <c r="B24" s="106" t="s">
         <v>97</v>
       </c>
       <c r="C24" s="59" t="s">
@@ -4615,7 +4466,7 @@
       <c r="A33" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="B33" s="103" t="s">
+      <c r="B33" s="106" t="s">
         <v>115</v>
       </c>
       <c r="C33" s="59" t="s">
@@ -4860,7 +4711,7 @@
       <c r="A53" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="B53" s="110" t="s">
+      <c r="B53" s="103" t="s">
         <v>156</v>
       </c>
       <c r="C53" s="59" t="s">
@@ -4913,7 +4764,7 @@
       <c r="A57" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="B57" s="103" t="s">
+      <c r="B57" s="106" t="s">
         <v>165</v>
       </c>
       <c r="C57" s="59" t="s">
@@ -4954,7 +4805,7 @@
       <c r="A60" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="B60" s="103" t="s">
+      <c r="B60" s="106" t="s">
         <v>172</v>
       </c>
       <c r="C60" s="59" t="s">
@@ -5163,7 +5014,7 @@
       <c r="A77" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="B77" s="110" t="s">
+      <c r="B77" s="103" t="s">
         <v>207</v>
       </c>
       <c r="C77" s="59" t="s">
@@ -5240,7 +5091,7 @@
       <c r="A83" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="B83" s="110" t="s">
+      <c r="B83" s="103" t="s">
         <v>220</v>
       </c>
       <c r="C83" s="59" t="s">
@@ -5305,7 +5156,7 @@
       <c r="A88" s="12" t="s">
         <v>230</v>
       </c>
-      <c r="B88" s="110" t="s">
+      <c r="B88" s="103" t="s">
         <v>231</v>
       </c>
       <c r="C88" s="59" t="s">
@@ -5346,7 +5197,7 @@
       <c r="A91" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="B91" s="110" t="s">
+      <c r="B91" s="103" t="s">
         <v>238</v>
       </c>
       <c r="C91" s="59" t="s">
@@ -5461,10 +5312,10 @@
     <row r="101" spans="1:6">
       <c r="A101" s="12"/>
       <c r="B101" s="64"/>
-      <c r="C101" s="111" t="s">
+      <c r="C101" s="105" t="s">
         <v>255</v>
       </c>
-      <c r="D101" s="111"/>
+      <c r="D101" s="105"/>
       <c r="E101" s="60"/>
       <c r="F101" s="53"/>
     </row>
@@ -5507,6 +5358,12 @@
   <sheetProtection algorithmName="SHA-512" hashValue="InmqKlhhVhE+dGbIYDiSRnLE+IlAZxdLfnctzqDZDARVCn6iziD6wICeby41lmvE4W1J88KUyAnY0y7x+sw6lQ==" saltValue="K8srq741x0YFfj6gj3u+2g==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="14">
+    <mergeCell ref="B33:B51"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B14:B22"/>
+    <mergeCell ref="B24:B31"/>
     <mergeCell ref="B91:B97"/>
     <mergeCell ref="C101:D101"/>
     <mergeCell ref="B53:B55"/>
@@ -5515,12 +5372,6 @@
     <mergeCell ref="B77:B81"/>
     <mergeCell ref="B83:B86"/>
     <mergeCell ref="B88:B89"/>
-    <mergeCell ref="B33:B51"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B14:B22"/>
-    <mergeCell ref="B24:B31"/>
   </mergeCells>
   <conditionalFormatting sqref="B23">
     <cfRule type="expression" dxfId="13" priority="13">
@@ -6223,7 +6074,7 @@
   <dimension ref="B1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6271,10 +6122,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="29"/>
-      <c r="F4" s="115" t="s">
+      <c r="F4" s="116" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="116"/>
+      <c r="G4" s="117"/>
       <c r="H4" s="1">
         <v>208</v>
       </c>
@@ -6283,10 +6134,10 @@
       </c>
     </row>
     <row r="5" spans="2:10" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1">
-      <c r="F5" s="117" t="s">
+      <c r="F5" s="118" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="118"/>
+      <c r="G5" s="119"/>
       <c r="H5" s="42">
         <v>8</v>
       </c>
@@ -6299,26 +6150,26 @@
       <c r="G6" s="40"/>
     </row>
     <row r="7" spans="2:10" ht="70" customHeight="1">
-      <c r="B7" s="112" t="s">
+      <c r="B7" s="114" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="19"/>
-      <c r="E7" s="119" t="s">
+      <c r="E7" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="119"/>
+      <c r="F7" s="120"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="120" t="s">
+      <c r="H7" s="112" t="s">
         <v>20</v>
       </c>
       <c r="J7"/>
     </row>
     <row r="8" spans="2:10" ht="26" customHeight="1">
-      <c r="B8" s="113"/>
-      <c r="H8" s="114"/>
+      <c r="B8" s="115"/>
+      <c r="H8" s="113"/>
       <c r="J8"/>
     </row>
     <row r="9" spans="2:10" ht="38.25" customHeight="1">
@@ -6335,7 +6186,7 @@
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="24">
-        <f>(C9*(VLOOKUP(E9,[1]Listes!$A$2:$B$5,2,FALSE))*VLOOKUP(F9,[1]Listes!$C$2:$D$6,2,FALSE))/($H$4*$C$3)</f>
+        <f>(C9*(VLOOKUP(E9,Listes!A2:B5,2,FALSE))*VLOOKUP(F9,Listes!C2:D6,2,FALSE))/($H$4*$C$3)</f>
         <v>0</v>
       </c>
       <c r="J9"/>
@@ -6355,7 +6206,7 @@
       <c r="J11"/>
     </row>
     <row r="12" spans="2:10" ht="69" customHeight="1">
-      <c r="B12" s="112" t="s">
+      <c r="B12" s="114" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="37" t="s">
@@ -6370,11 +6221,11 @@
       <c r="J12"/>
     </row>
     <row r="13" spans="2:10" ht="34.5" customHeight="1">
-      <c r="B13" s="113"/>
+      <c r="B13" s="115"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="9"/>
-      <c r="G13" s="114" t="s">
+      <c r="G13" s="113" t="s">
         <v>21</v>
       </c>
       <c r="J13"/>
@@ -6388,7 +6239,7 @@
       <c r="E14" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="114"/>
+      <c r="G14" s="113"/>
     </row>
     <row r="15" spans="2:10" s="3" customFormat="1" ht="6.75" customHeight="1">
       <c r="B15" s="17"/>
@@ -6407,7 +6258,7 @@
         <v>6</v>
       </c>
       <c r="G16" s="24">
-        <f>(C14*VLOOKUP(E14,[1]Listes!A2:B5,2,FALSE))*C16*VLOOKUP(E16,[1]Listes!C2:D6,2,FALSE)/($H$4*$C$3)</f>
+        <f>(C14*VLOOKUP(E14,Listes!A2:B5,2,FALSE))*C16*VLOOKUP(E16,Listes!C2:D6,2,FALSE)/($H$4*$C$3)</f>
         <v>0</v>
       </c>
     </row>
@@ -6432,7 +6283,7 @@
       <c r="D19" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="UPLbUm1+bqbfXmnMLcE8Rn9CI/NBcf5Up43OtNldliMyg6/LXkybQr77PYuL6n+coy8Bh+riYhCBrKUx4lshFg==" saltValue="IIHMr8JbSN/brD69Lfg/dg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="cKM2N5HkSDHgCijs1RU8KsRCjv88tQS0Hu+Cmq/Xf2lBsOIEHYy9oGF2Elf5DzuqKZRHPRjvKsCE0meKMf6oBg==" saltValue="T7NWVPg98zc1GEY7hA5pPQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="7">
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="B12:B13"/>
@@ -6483,7 +6334,7 @@
   <dimension ref="B1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6533,10 +6384,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="29"/>
-      <c r="F4" s="115" t="s">
+      <c r="F4" s="116" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="116"/>
+      <c r="G4" s="117"/>
       <c r="H4" s="1">
         <v>1607</v>
       </c>
@@ -6545,10 +6396,10 @@
       </c>
     </row>
     <row r="5" spans="2:10" s="3" customFormat="1" ht="24.75" customHeight="1" thickBot="1">
-      <c r="F5" s="117" t="s">
+      <c r="F5" s="118" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="118"/>
+      <c r="G5" s="119"/>
       <c r="H5" s="39">
         <v>35</v>
       </c>
@@ -6563,26 +6414,26 @@
       </c>
     </row>
     <row r="7" spans="2:10" ht="70" customHeight="1">
-      <c r="B7" s="112" t="s">
+      <c r="B7" s="114" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="19"/>
-      <c r="E7" s="119" t="s">
+      <c r="E7" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="119"/>
+      <c r="F7" s="120"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="120" t="s">
+      <c r="H7" s="112" t="s">
         <v>20</v>
       </c>
       <c r="J7"/>
     </row>
     <row r="8" spans="2:10" ht="26" customHeight="1">
-      <c r="B8" s="113"/>
-      <c r="H8" s="114"/>
+      <c r="B8" s="115"/>
+      <c r="H8" s="113"/>
       <c r="J8"/>
     </row>
     <row r="9" spans="2:10" ht="38.25" customHeight="1">
@@ -6599,7 +6450,7 @@
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="24">
-        <f>(C9*(VLOOKUP(E9,[1]Listes!$A$9:$B$12,2,FALSE))*VLOOKUP(F9,[1]Listes!$C$9:$D$13,2,FALSE))/(($H$4)*$C$3)</f>
+        <f>(C9*(VLOOKUP(E9,Listes!A9:B12,2,FALSE))*VLOOKUP(F9,Listes!C9:D13,2,FALSE))/(($H$4)*$C$3)</f>
         <v>0</v>
       </c>
       <c r="J9"/>
@@ -6619,7 +6470,7 @@
       <c r="J11"/>
     </row>
     <row r="12" spans="2:10" ht="69" customHeight="1">
-      <c r="B12" s="112" t="s">
+      <c r="B12" s="114" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="37" t="s">
@@ -6634,11 +6485,11 @@
       <c r="J12"/>
     </row>
     <row r="13" spans="2:10" ht="34.5" customHeight="1">
-      <c r="B13" s="113"/>
+      <c r="B13" s="115"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="9"/>
-      <c r="G13" s="114" t="s">
+      <c r="G13" s="113" t="s">
         <v>21</v>
       </c>
       <c r="J13"/>
@@ -6652,7 +6503,7 @@
       <c r="E14" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="114"/>
+      <c r="G14" s="113"/>
     </row>
     <row r="15" spans="2:10" s="3" customFormat="1" ht="6.75" customHeight="1">
       <c r="B15" s="17"/>
@@ -6671,7 +6522,7 @@
         <v>6</v>
       </c>
       <c r="G16" s="24">
-        <f>(C14*VLOOKUP(E14,[1]Listes!A9:B12,2,FALSE))*C16*VLOOKUP(E16,[1]Listes!C9:D13,2,FALSE)/($H$4*$C$3)</f>
+        <f>(C14*VLOOKUP(E14,Listes!A9:B12,2,FALSE))*C16*VLOOKUP(E16,Listes!C9:D13,2,FALSE)/($H$4*$C$3)</f>
         <v>0</v>
       </c>
     </row>
@@ -6696,7 +6547,7 @@
       <c r="D19" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="3niYrB0o6qf6v+PSHMrO4Z/NUX5mRFNdVO+Yrc0OkSXoAXux8c7HqMx5VlRPv+WUh+Y9LCyMSAHO8F9VRIQvtQ==" saltValue="MHmavSrorJTb/4/9UqPOLA==" spinCount="100000" sheet="1" objects="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="gN68Zzzpydn61AAvwV9vxthhrTLlrzkWyfWXe0z4fbajxSdNTR1j8ndJGhE3OPwJbmdb0KsoCIJo2NEvrtEV3w==" saltValue="0YnQ7WvC9cJKx2J0NhS59w==" spinCount="100000" sheet="1" objects="1" selectLockedCells="1"/>
   <mergeCells count="8">
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="G13:G14"/>
@@ -6861,7 +6712,7 @@
         <v>45</v>
       </c>
       <c r="D11" s="85">
-        <f>IF(D3="MAGISTRAT",D6*D8*[1]Listes!D3,D6*D8*[1]Fonctionnaires!H4/7)</f>
+        <f>IF(D3="MAGISTRAT",D6*D8*Listes!D3,D6*D8*'Calculatrice - Fonctionnaires'!H4/7)</f>
         <v>0</v>
       </c>
       <c r="E11" s="86" t="s">
@@ -6893,59 +6744,59 @@
       <c r="F12" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="92">
+      <c r="G12" s="91">
         <f>IF(D4="FONCTIONNAIRE",D12*7,D12*8)</f>
         <v>0</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="I12" s="93"/>
+      <c r="I12" s="92"/>
     </row>
     <row r="13" spans="3:9" ht="24" customHeight="1">
-      <c r="C13" s="94" t="s">
+      <c r="C13" s="93" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="95">
+      <c r="D13" s="94">
         <f>(D8*D6)*5</f>
         <v>0</v>
       </c>
-      <c r="E13" s="96" t="s">
+      <c r="E13" s="95" t="s">
         <v>362</v>
       </c>
-      <c r="F13" s="97" t="s">
+      <c r="F13" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="98">
+      <c r="G13" s="97">
         <f>IF(D3="FONCTIONNAIRE",D13*7,D13*8)</f>
         <v>0</v>
       </c>
-      <c r="H13" s="96" t="s">
+      <c r="H13" s="95" t="s">
         <v>363</v>
       </c>
-      <c r="I13" s="99"/>
+      <c r="I13" s="98"/>
     </row>
     <row r="14" spans="3:9" ht="16.25" customHeight="1">
-      <c r="C14" s="100" t="s">
+      <c r="C14" s="99" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="15" spans="3:9" ht="16.25" customHeight="1">
-      <c r="C15" s="100" t="s">
+      <c r="C15" s="99" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="16" spans="3:9" ht="24" customHeight="1">
-      <c r="C16" s="101"/>
+      <c r="C16" s="100"/>
     </row>
     <row r="17" spans="3:3" ht="24" customHeight="1">
-      <c r="C17" s="102"/>
+      <c r="C17" s="101"/>
     </row>
     <row r="18" spans="3:3" ht="24" customHeight="1">
-      <c r="C18" s="101"/>
+      <c r="C18" s="100"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="aDXNkJ2efhryHHrInatlkZ3y7C07jmVd4jT9/If0kG3duKVA++0b+Qvz89QqdJ++xH35TQ5tb2xjeV5Kx2n8iQ==" saltValue="KteL1vZhNZpNVuhiO2P9Vg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="LPGke7/ZH4S+bl7gS7AmrYxN7a2y0svDE8sTZW7XcdKX17IuH7HwrmxdTykh25OvdZ6VQDlSWjhfUfePOg6/pQ==" saltValue="z44X+kRlscZ2QAMWEkQsxw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="3">
     <mergeCell ref="C2:I2"/>
     <mergeCell ref="D3:E3"/>
@@ -6974,7 +6825,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -7006,7 +6857,7 @@
         <v>27</v>
       </c>
       <c r="D3">
-        <f>[2]Magistrats!H4</f>
+        <f>[1]Magistrats!H4</f>
         <v>208</v>
       </c>
       <c r="F3" t="s">
@@ -7033,7 +6884,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <f>1/[2]Magistrats!H5</f>
+        <f>1/[1]Magistrats!H5</f>
         <v>0.125</v>
       </c>
       <c r="C5" t="s">
@@ -7071,14 +6922,14 @@
         <v>1</v>
       </c>
       <c r="B10" s="38">
-        <f>[2]Fonctionnaires!H5/5</f>
+        <f>[1]Fonctionnaires!H5/5</f>
         <v>7</v>
       </c>
       <c r="C10" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="38">
-        <f>[2]Fonctionnaires!H4/[2]Listes!B10</f>
+        <f>[1]Fonctionnaires!H4/[1]Listes!B10</f>
         <v>229.57142857142858</v>
       </c>
     </row>
@@ -7094,7 +6945,7 @@
         <v>28</v>
       </c>
       <c r="D11" s="38">
-        <f>[2]Fonctionnaires!H4/[2]Fonctionnaires!H5</f>
+        <f>[1]Fonctionnaires!H4/[1]Fonctionnaires!H5</f>
         <v>45.914285714285711</v>
       </c>
     </row>
@@ -7123,12 +6974,12 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="16">
-      <c r="A15" s="128" t="s">
+      <c r="A15" s="102" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16">
-      <c r="A16" s="128" t="s">
+      <c r="A16" s="102" t="s">
         <v>366</v>
       </c>
     </row>

</xml_diff>